<commit_message>
EUR 1M YC - first cut
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -2871,7 +2871,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="89">
-        <v>41628.427523148152</v>
+        <v>41628.428842592592</v>
       </c>
       <c r="E11" s="61"/>
       <c r="F11" s="60"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="D14" s="86" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC1M#0001</v>
+        <v>_EURYC1M#0002</v>
       </c>
       <c r="E14" s="61"/>
       <c r="F14" s="60"/>
@@ -12442,7 +12442,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_RateHelpersSelected#0001</v>
+        <v>EUR_YC1MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="44" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -15587,7 +15587,7 @@
       </c>
       <c r="F3" s="114" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_SND#0002</v>
+        <v>EUR_YC1MRH_SND#0003</v>
       </c>
       <c r="G3" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -15614,7 +15614,7 @@
       </c>
       <c r="F4" s="108" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_SWD#0002</v>
+        <v>EUR_YC1MRH_SWD#0003</v>
       </c>
       <c r="G4" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -15641,7 +15641,7 @@
       </c>
       <c r="F5" s="108" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2WD#0002</v>
+        <v>EUR_YC1MRH_2WD#0003</v>
       </c>
       <c r="G5" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -15668,7 +15668,7 @@
       </c>
       <c r="F6" s="108" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3WD#0002</v>
+        <v>EUR_YC1MRH_3WD#0003</v>
       </c>
       <c r="G6" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -15695,7 +15695,7 @@
       </c>
       <c r="F7" s="108" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_1MD#0002</v>
+        <v>EUR_YC1MRH_1MD#0003</v>
       </c>
       <c r="G7" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -15844,7 +15844,7 @@
       </c>
       <c r="L4" s="157" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1MRH_xX1S_ibor1M#0002</v>
+        <v>EUR_YC1MRH_xX1S_ibor1M#0003</v>
       </c>
       <c r="M4" s="156" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -15905,7 +15905,7 @@
       </c>
       <c r="L6" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2X1S#0002</v>
+        <v>EUR_YC1MRH_2X1S#0003</v>
       </c>
       <c r="M6" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -15950,7 +15950,7 @@
       </c>
       <c r="L7" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3X1S#0002</v>
+        <v>EUR_YC1MRH_3X1S#0003</v>
       </c>
       <c r="M7" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -15995,7 +15995,7 @@
       </c>
       <c r="L8" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_4X1S#0002</v>
+        <v>EUR_YC1MRH_4X1S#0003</v>
       </c>
       <c r="M8" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -16040,7 +16040,7 @@
       </c>
       <c r="L9" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_5X1S#0002</v>
+        <v>EUR_YC1MRH_5X1S#0003</v>
       </c>
       <c r="M9" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -16085,7 +16085,7 @@
       </c>
       <c r="L10" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_6X1S#0002</v>
+        <v>EUR_YC1MRH_6X1S#0003</v>
       </c>
       <c r="M10" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="L11" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_7X1S#0002</v>
+        <v>EUR_YC1MRH_7X1S#0003</v>
       </c>
       <c r="M11" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -16175,7 +16175,7 @@
       </c>
       <c r="L12" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_8X1S#0002</v>
+        <v>EUR_YC1MRH_8X1S#0003</v>
       </c>
       <c r="M12" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -16220,7 +16220,7 @@
       </c>
       <c r="L13" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_9X1S#0002</v>
+        <v>EUR_YC1MRH_9X1S#0003</v>
       </c>
       <c r="M13" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -16265,7 +16265,7 @@
       </c>
       <c r="L14" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_10X1S#0002</v>
+        <v>EUR_YC1MRH_10X1S#0003</v>
       </c>
       <c r="M14" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -16310,7 +16310,7 @@
       </c>
       <c r="L15" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_11X1S#0002</v>
+        <v>EUR_YC1MRH_11X1S#0003</v>
       </c>
       <c r="M15" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -16355,7 +16355,7 @@
       </c>
       <c r="L16" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_12X1S#0002</v>
+        <v>EUR_YC1MRH_12X1S#0003</v>
       </c>
       <c r="M16" s="116" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -16536,7 +16536,7 @@
       </c>
       <c r="L4" s="157" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1MRH_AB1EBASIS_ibor1M#0002</v>
+        <v>EUR_YC1MRH_AB1EBASIS_ibor1M#0003</v>
       </c>
       <c r="M4" s="156" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -16600,7 +16600,7 @@
       </c>
       <c r="L6" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS1Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS1Y#0002</v>
       </c>
       <c r="M6" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -16649,7 +16649,7 @@
       </c>
       <c r="L7" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS15M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15M#0002</v>
       </c>
       <c r="M7" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -16698,7 +16698,7 @@
       </c>
       <c r="L8" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS18M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18M#0002</v>
       </c>
       <c r="M8" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -16747,7 +16747,7 @@
       </c>
       <c r="L9" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS21M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21M#0002</v>
       </c>
       <c r="M9" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -16796,7 +16796,7 @@
       </c>
       <c r="L10" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS2Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS2Y#0002</v>
       </c>
       <c r="M10" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -16854,7 +16854,7 @@
       </c>
       <c r="L11" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS3Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS3Y#0002</v>
       </c>
       <c r="M11" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -16912,7 +16912,7 @@
       </c>
       <c r="L12" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS4Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS4Y#0002</v>
       </c>
       <c r="M12" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -16970,7 +16970,7 @@
       </c>
       <c r="L13" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS5Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS5Y#0002</v>
       </c>
       <c r="M13" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -17028,7 +17028,7 @@
       </c>
       <c r="L14" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS6Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS6Y#0002</v>
       </c>
       <c r="M14" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -17086,7 +17086,7 @@
       </c>
       <c r="L15" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS7Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS7Y#0002</v>
       </c>
       <c r="M15" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -17138,7 +17138,7 @@
       </c>
       <c r="L16" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS8Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS8Y#0002</v>
       </c>
       <c r="M16" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -17187,7 +17187,7 @@
       </c>
       <c r="L17" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS9Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS9Y#0002</v>
       </c>
       <c r="M17" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -17236,7 +17236,7 @@
       </c>
       <c r="L18" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS10Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS10Y#0002</v>
       </c>
       <c r="M18" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -17285,7 +17285,7 @@
       </c>
       <c r="L19" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS11Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS11Y#0002</v>
       </c>
       <c r="M19" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -17334,7 +17334,7 @@
       </c>
       <c r="L20" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS12Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS12Y#0002</v>
       </c>
       <c r="M20" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -17383,7 +17383,7 @@
       </c>
       <c r="L21" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS13Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS13Y#0002</v>
       </c>
       <c r="M21" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -17432,7 +17432,7 @@
       </c>
       <c r="L22" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS14Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS14Y#0002</v>
       </c>
       <c r="M22" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -17481,7 +17481,7 @@
       </c>
       <c r="L23" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS15Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15Y#0002</v>
       </c>
       <c r="M23" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -17530,7 +17530,7 @@
       </c>
       <c r="L24" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS16Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS16Y#0002</v>
       </c>
       <c r="M24" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -17579,7 +17579,7 @@
       </c>
       <c r="L25" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS17Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS17Y#0002</v>
       </c>
       <c r="M25" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -17628,7 +17628,7 @@
       </c>
       <c r="L26" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS18Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18Y#0002</v>
       </c>
       <c r="M26" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -17677,7 +17677,7 @@
       </c>
       <c r="L27" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS19Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS19Y#0002</v>
       </c>
       <c r="M27" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -17726,7 +17726,7 @@
       </c>
       <c r="L28" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS20Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS20Y#0002</v>
       </c>
       <c r="M28" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -17775,7 +17775,7 @@
       </c>
       <c r="L29" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS21Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21Y#0002</v>
       </c>
       <c r="M29" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -17824,7 +17824,7 @@
       </c>
       <c r="L30" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS22Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS22Y#0002</v>
       </c>
       <c r="M30" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -17873,7 +17873,7 @@
       </c>
       <c r="L31" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS23Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS23Y#0002</v>
       </c>
       <c r="M31" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -17922,7 +17922,7 @@
       </c>
       <c r="L32" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS24Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS24Y#0002</v>
       </c>
       <c r="M32" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -17971,7 +17971,7 @@
       </c>
       <c r="L33" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS25Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS25Y#0002</v>
       </c>
       <c r="M33" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -18020,7 +18020,7 @@
       </c>
       <c r="L34" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS26Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS26Y#0002</v>
       </c>
       <c r="M34" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -18069,7 +18069,7 @@
       </c>
       <c r="L35" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS27Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS27Y#0002</v>
       </c>
       <c r="M35" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -18118,7 +18118,7 @@
       </c>
       <c r="L36" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS28Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS28Y#0002</v>
       </c>
       <c r="M36" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -18167,7 +18167,7 @@
       </c>
       <c r="L37" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS29Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS29Y#0002</v>
       </c>
       <c r="M37" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -18216,7 +18216,7 @@
       </c>
       <c r="L38" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS30Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS30Y#0002</v>
       </c>
       <c r="M38" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -18265,7 +18265,7 @@
       </c>
       <c r="L39" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS35Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS35Y#0002</v>
       </c>
       <c r="M39" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -18314,7 +18314,7 @@
       </c>
       <c r="L40" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS40Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS40Y#0002</v>
       </c>
       <c r="M40" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -18363,7 +18363,7 @@
       </c>
       <c r="L41" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS50Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS50Y#0002</v>
       </c>
       <c r="M41" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -18412,7 +18412,7 @@
       </c>
       <c r="L42" s="149" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS60Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS60Y#0002</v>
       </c>
       <c r="M42" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>

<commit_message>
reconcile with R010202 prod
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="199">
   <si>
     <t>60Y</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>EUR_YC1MRH_SND</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1481,7 @@
     <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1873,6 +1876,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2389,7 +2393,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="87">
-        <v>41632.2497337963</v>
+        <v>41662.585138888891</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="58"/>
@@ -2444,7 +2448,7 @@
       </c>
       <c r="D14" s="84" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC1M#0007</v>
+        <v>_EURYC1M#0000</v>
       </c>
       <c r="E14" s="59"/>
       <c r="F14" s="58"/>
@@ -2557,11 +2561,11 @@
       </c>
       <c r="D21" s="76">
         <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
-        <v>41639</v>
+        <v>42004</v>
       </c>
       <c r="E21" s="75">
         <f>DATE(YEAR(D21+1),12,31)</f>
-        <v>42004</v>
+        <v>42369</v>
       </c>
       <c r="F21" s="58"/>
     </row>
@@ -2625,7 +2629,7 @@
       <c r="B27" s="62"/>
       <c r="C27" s="66">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="D27" s="65">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2638,11 +2642,11 @@
       <c r="B28" s="62"/>
       <c r="C28" s="64">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>63552</v>
+        <v>63576</v>
       </c>
       <c r="D28" s="63">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.20786045634669514</v>
+        <v>0.20792736615750362</v>
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="58"/>
@@ -2869,11 +2873,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41639</v>
+        <v>41661</v>
       </c>
       <c r="M4" s="1">
         <v>30</v>
@@ -2908,11 +2912,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41645</v>
+        <v>41667</v>
       </c>
       <c r="M5" s="1">
         <v>40</v>
@@ -2947,11 +2951,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41652</v>
+        <v>41674</v>
       </c>
       <c r="M6" s="1">
         <v>50</v>
@@ -2986,11 +2990,11 @@
       </c>
       <c r="K7" s="11">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L7" s="10">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41659</v>
+        <v>41681</v>
       </c>
       <c r="M7" s="1">
         <v>60</v>
@@ -3025,11 +3029,11 @@
       </c>
       <c r="K8" s="11">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L8" s="10">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41669</v>
+        <v>41691</v>
       </c>
       <c r="M8" s="1">
         <v>70</v>
@@ -4043,11 +4047,11 @@
       </c>
       <c r="D36" s="14" t="str">
         <f t="array" ref="D36:D77">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A36:$A77)</f>
-        <v>F4</v>
+        <v>G4</v>
       </c>
       <c r="E36" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MF4</v>
+        <v>EUR_YC1MRH_FUT1MG4</v>
       </c>
       <c r="F36" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -4085,11 +4089,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D37" s="14" t="str">
-        <v>G4</v>
+        <v>H4</v>
       </c>
       <c r="E37" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MG4</v>
+        <v>EUR_YC1MRH_FUT1MH4</v>
       </c>
       <c r="F37" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4127,11 +4131,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D38" s="14" t="str">
-        <v>H4</v>
+        <v>J4</v>
       </c>
       <c r="E38" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH4</v>
+        <v>EUR_YC1MRH_FUT1MJ4</v>
       </c>
       <c r="F38" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4169,11 +4173,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D39" s="14" t="str">
-        <v>J4</v>
+        <v>K4</v>
       </c>
       <c r="E39" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MJ4</v>
+        <v>EUR_YC1MRH_FUT1MK4</v>
       </c>
       <c r="F39" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4211,11 +4215,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D40" s="14" t="str">
-        <v>K4</v>
+        <v>M4</v>
       </c>
       <c r="E40" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MK4</v>
+        <v>EUR_YC1MRH_FUT1MM4</v>
       </c>
       <c r="F40" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4253,11 +4257,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D41" s="14" t="str">
-        <v>M4</v>
+        <v>N4</v>
       </c>
       <c r="E41" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM4</v>
+        <v>EUR_YC1MRH_FUT1MN4</v>
       </c>
       <c r="F41" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4295,11 +4299,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D42" s="14" t="str">
-        <v>N4</v>
+        <v>Q4</v>
       </c>
       <c r="E42" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MN4</v>
+        <v>EUR_YC1MRH_FUT1MQ4</v>
       </c>
       <c r="F42" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4337,11 +4341,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D43" s="14" t="str">
-        <v>Q4</v>
+        <v>U4</v>
       </c>
       <c r="E43" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MQ4</v>
+        <v>EUR_YC1MRH_FUT1MU4</v>
       </c>
       <c r="F43" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4379,11 +4383,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D44" s="14" t="str">
-        <v>U4</v>
+        <v>V4</v>
       </c>
       <c r="E44" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU4</v>
+        <v>EUR_YC1MRH_FUT1MV4</v>
       </c>
       <c r="F44" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4421,11 +4425,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D45" s="14" t="str">
-        <v>V4</v>
+        <v>X4</v>
       </c>
       <c r="E45" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MV4</v>
+        <v>EUR_YC1MRH_FUT1MX4</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4463,11 +4467,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D46" s="14" t="str">
-        <v>X4</v>
+        <v>Z4</v>
       </c>
       <c r="E46" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MX4</v>
+        <v>EUR_YC1MRH_FUT1MZ4</v>
       </c>
       <c r="F46" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4505,11 +4509,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D47" s="14" t="str">
-        <v>Z4</v>
+        <v>F5</v>
       </c>
       <c r="E47" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ4</v>
+        <v>EUR_YC1MRH_FUT1MF5</v>
       </c>
       <c r="F47" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -5829,11 +5833,11 @@
       </c>
       <c r="K78" s="18">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L78" s="17">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>41698</v>
+        <v>41719</v>
       </c>
       <c r="M78" s="22"/>
     </row>
@@ -5868,11 +5872,11 @@
       </c>
       <c r="K79" s="11">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L79" s="10">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>41729</v>
+        <v>41751</v>
       </c>
       <c r="M79" s="25"/>
     </row>
@@ -5907,11 +5911,11 @@
       </c>
       <c r="K80" s="11">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L80" s="10">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>41759</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
@@ -5945,11 +5949,11 @@
       </c>
       <c r="K81" s="11">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L81" s="10">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>41789</v>
+        <v>41813</v>
       </c>
     </row>
     <row r="82" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5983,11 +5987,11 @@
       </c>
       <c r="K82" s="11">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L82" s="10">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>41820</v>
+        <v>41841</v>
       </c>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.2">
@@ -6021,11 +6025,11 @@
       </c>
       <c r="K83" s="11">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L83" s="10">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>41850</v>
+        <v>41872</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
@@ -6059,11 +6063,11 @@
       </c>
       <c r="K84" s="11">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L84" s="10">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>41880</v>
+        <v>41904</v>
       </c>
     </row>
     <row r="85" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6097,11 +6101,11 @@
       </c>
       <c r="K85" s="11">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L85" s="10">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>41912</v>
+        <v>41933</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
@@ -6135,11 +6139,11 @@
       </c>
       <c r="K86" s="11">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L86" s="10">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>41942</v>
+        <v>41964</v>
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
@@ -6173,11 +6177,11 @@
       </c>
       <c r="K87" s="11">
         <f>_xll.qlRateHelperEarliestDate($E87,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L87" s="10">
         <f>_xll.qlRateHelperLatestDate($E87,Trigger)</f>
-        <v>41971</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.2">
@@ -6211,11 +6215,11 @@
       </c>
       <c r="K88" s="4">
         <f>_xll.qlRateHelperEarliestDate($E88,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L88" s="3">
         <f>_xll.qlRateHelperLatestDate($E88,Trigger)</f>
-        <v>42003</v>
+        <v>42025</v>
       </c>
     </row>
     <row r="89" spans="2:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8061,7 +8065,7 @@
         <v>2</v>
       </c>
       <c r="E130" s="14" t="str">
-        <f t="shared" ref="E130:E161" si="10">RateHelperPrefix&amp;"_"&amp;$B130&amp;$C130&amp;$D130</f>
+        <f t="shared" ref="E130:E132" si="10">RateHelperPrefix&amp;"_"&amp;$B130&amp;$C130&amp;$D130</f>
         <v>EUR_YC1MRH_AB1E40Y</v>
       </c>
       <c r="F130" s="13" t="e">
@@ -8221,11 +8225,11 @@
       </c>
       <c r="K133" s="18">
         <f>_xll.qlRateHelperEarliestDate($E133,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L133" s="17">
         <f>_xll.qlRateHelperLatestDate($E133,Trigger)</f>
-        <v>42003</v>
+        <v>42025</v>
       </c>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.2">
@@ -8263,11 +8267,11 @@
       </c>
       <c r="K134" s="11">
         <f>_xll.qlRateHelperEarliestDate($E134,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L134" s="10">
         <f>_xll.qlRateHelperLatestDate($E134,Trigger)</f>
-        <v>42093</v>
+        <v>42115</v>
       </c>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.2">
@@ -8305,11 +8309,11 @@
       </c>
       <c r="K135" s="11">
         <f>_xll.qlRateHelperEarliestDate($E135,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L135" s="10">
         <f>_xll.qlRateHelperLatestDate($E135,Trigger)</f>
-        <v>42185</v>
+        <v>42206</v>
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.2">
@@ -8347,11 +8351,11 @@
       </c>
       <c r="K136" s="11">
         <f>_xll.qlRateHelperEarliestDate($E136,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L136" s="10">
         <f>_xll.qlRateHelperLatestDate($E136,Trigger)</f>
-        <v>42277</v>
+        <v>42298</v>
       </c>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.2">
@@ -8389,11 +8393,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>42368</v>
+        <v>42390</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8431,11 +8435,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>42734</v>
+        <v>42758</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8473,11 +8477,11 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>43098</v>
+        <v>43122</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
@@ -8515,11 +8519,11 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>43465</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
@@ -8557,11 +8561,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>43829</v>
+        <v>43851</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8599,11 +8603,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>44195</v>
+        <v>44217</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8641,11 +8645,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>44560</v>
+        <v>44582</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8683,11 +8687,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>44925</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8725,11 +8729,11 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>45289</v>
+        <v>45313</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
@@ -8767,11 +8771,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>45656</v>
+        <v>45678</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8809,11 +8813,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46021</v>
+        <v>46043</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8851,11 +8855,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>46386</v>
+        <v>46408</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8893,11 +8897,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>46751</v>
+        <v>46773</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8935,11 +8939,11 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>47116</v>
+        <v>47140</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
@@ -8977,11 +8981,11 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>47483</v>
+        <v>47504</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
@@ -9019,11 +9023,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>47847</v>
+        <v>47869</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -9061,11 +9065,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>48212</v>
+        <v>48234</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -9103,11 +9107,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>48578</v>
+        <v>48600</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9145,11 +9149,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>48943</v>
+        <v>48967</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9187,11 +9191,11 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>49307</v>
+        <v>49331</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
@@ -9229,11 +9233,11 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>49674</v>
+        <v>49695</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
@@ -9271,11 +9275,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50039</v>
+        <v>50061</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9313,11 +9317,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>50404</v>
+        <v>50426</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9355,11 +9359,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>50769</v>
+        <v>50791</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9397,11 +9401,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>51134</v>
+        <v>51158</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9439,11 +9443,11 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>51501</v>
+        <v>51522</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.2">
@@ -9481,11 +9485,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>51865</v>
+        <v>51887</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9523,11 +9527,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>52230</v>
+        <v>52252</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9565,11 +9569,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>52595</v>
+        <v>52617</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9607,11 +9611,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>54422</v>
+        <v>54444</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9649,11 +9653,11 @@
       </c>
       <c r="K167" s="11">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L167" s="10">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>56248</v>
+        <v>56270</v>
       </c>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.2">
@@ -9691,11 +9695,11 @@
       </c>
       <c r="K168" s="11">
         <f>_xll.qlRateHelperEarliestDate($E168,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L168" s="10">
         <f>_xll.qlRateHelperLatestDate($E168,Trigger)</f>
-        <v>59901</v>
+        <v>59922</v>
       </c>
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.2">
@@ -9733,11 +9737,11 @@
       </c>
       <c r="K169" s="4">
         <f>_xll.qlRateHelperEarliestDate($E169,Trigger)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="L169" s="3">
         <f>_xll.qlRateHelperLatestDate($E169,Trigger)</f>
-        <v>63552</v>
+        <v>63576</v>
       </c>
     </row>
   </sheetData>
@@ -9820,20 +9824,20 @@
       </c>
       <c r="G2" s="40">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H2" s="39">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41639</v>
+        <v>41661</v>
       </c>
       <c r="I2" s="34">
         <v>0.99999652778983417</v>
       </c>
       <c r="K2" s="92" t="s">
-        <v>116</v>
+        <v>198</v>
       </c>
       <c r="L2" s="93">
-        <v>1.33E-3</v>
+        <v>2.8939999999999999E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -9856,20 +9860,20 @@
       </c>
       <c r="G3" s="40">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H3" s="39">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41645</v>
+        <v>41667</v>
       </c>
       <c r="I3" s="34">
         <v>0.99997413955766812</v>
       </c>
       <c r="K3" s="92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L3" s="93">
-        <v>1.31E-3</v>
+        <v>2.3930000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -9892,20 +9896,20 @@
       </c>
       <c r="G4" s="40">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H4" s="39">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41652</v>
+        <v>41674</v>
       </c>
       <c r="I4" s="34">
         <v>0.99994905815077162</v>
       </c>
       <c r="K4" s="92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L4" s="93">
-        <v>1.31E-3</v>
+        <v>2.513E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -9928,20 +9932,20 @@
       </c>
       <c r="G5" s="40">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H5" s="39">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41659</v>
+        <v>41681</v>
       </c>
       <c r="I5" s="34">
         <v>0.99992358917239399</v>
       </c>
       <c r="K5" s="92" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="93">
-        <v>1.31E-3</v>
+        <v>2.4629999999999999E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -9965,26 +9969,26 @@
       </c>
       <c r="G6" s="40">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H6" s="39">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41669</v>
+        <v>41691</v>
       </c>
       <c r="I6" s="34">
         <v>0.99988720716810242</v>
       </c>
       <c r="K6" s="92" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="93">
-        <v>1.3600000000000001E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_RateHelpersSelected#0007</v>
+        <v>EUR_YC1MRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="44" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10003,20 +10007,20 @@
       </c>
       <c r="G7" s="40">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H7" s="39">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41698</v>
+        <v>41719</v>
       </c>
       <c r="I7" s="34">
-        <v>0.99977338469956589</v>
+        <v>0.99977716077963408</v>
       </c>
       <c r="K7" s="92" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L7" s="93">
-        <v>1.4200000000000003E-3</v>
+        <v>2.4099999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -10033,20 +10037,20 @@
       </c>
       <c r="G8" s="40">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H8" s="39">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41729</v>
+        <v>41751</v>
       </c>
       <c r="I8" s="34">
         <v>0.99964118435043958</v>
       </c>
       <c r="K8" s="92" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L8" s="93">
-        <v>1.4600000000000001E-3</v>
+        <v>2.33E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -10063,20 +10067,20 @@
       </c>
       <c r="G9" s="40">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H9" s="39">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41759</v>
+        <v>41780</v>
       </c>
       <c r="I9" s="34">
-        <v>0.9995095184679651</v>
+        <v>0.99951357006256958</v>
       </c>
       <c r="K9" s="92" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L9" s="93">
-        <v>1.5100000000000001E-3</v>
+        <v>2.2399999999999998E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -10093,20 +10097,20 @@
       </c>
       <c r="G10" s="40">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41789</v>
+        <v>41813</v>
       </c>
       <c r="I10" s="34">
-        <v>0.99936703978127628</v>
+        <v>0.99935866157893161</v>
       </c>
       <c r="K10" s="92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L10" s="93">
-        <v>1.58E-3</v>
+        <v>2.1800000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -10123,20 +10127,20 @@
       </c>
       <c r="G11" s="40">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41820</v>
+        <v>41841</v>
       </c>
       <c r="I11" s="34">
-        <v>0.9992018597589104</v>
+        <v>0.99920624166391381</v>
       </c>
       <c r="K11" s="92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L11" s="93">
-        <v>1.6300000000000002E-3</v>
+        <v>2.14E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -10153,20 +10157,20 @@
       </c>
       <c r="G12" s="40">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41850</v>
+        <v>41872</v>
       </c>
       <c r="I12" s="34">
-        <v>0.99904103161420943</v>
+        <v>0.99904103161420954</v>
       </c>
       <c r="K12" s="92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L12" s="93">
-        <v>1.6999999999999999E-3</v>
+        <v>2.1199999999999999E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -10183,20 +10187,20 @@
       </c>
       <c r="G13" s="40">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>41880</v>
+        <v>41904</v>
       </c>
       <c r="I13" s="34">
-        <v>0.9988652336021151</v>
+        <v>0.9988558660973782</v>
       </c>
       <c r="K13" s="92" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L13" s="93">
-        <v>1.7899999999999999E-3</v>
+        <v>2.1099999999999999E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -10213,20 +10217,20 @@
       </c>
       <c r="G14" s="40">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>41912</v>
+        <v>41933</v>
       </c>
       <c r="I14" s="34">
-        <v>0.99863946468930165</v>
+        <v>0.99864442341558202</v>
       </c>
       <c r="K14" s="92" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L14" s="93">
-        <v>1.8599999999999999E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -10243,20 +10247,20 @@
       </c>
       <c r="G15" s="40">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>41942</v>
+        <v>41964</v>
       </c>
       <c r="I15" s="34">
         <v>0.99843179645836277</v>
       </c>
       <c r="K15" s="92" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L15" s="93">
-        <v>1.9500000000000001E-3</v>
+        <v>2.0799999999999998E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -10273,20 +10277,20 @@
       </c>
       <c r="G16" s="40">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>41971</v>
+        <v>41995</v>
       </c>
       <c r="I16" s="34">
-        <v>0.99819949765610294</v>
+        <v>0.99818870341526134</v>
       </c>
       <c r="K16" s="92" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L16" s="93">
-        <v>2.0400000000000001E-3</v>
+        <v>2.0699999999999998E-3</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
@@ -10303,20 +10307,20 @@
       </c>
       <c r="G17" s="40">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H17" s="39">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42003</v>
+        <v>42025</v>
       </c>
       <c r="I17" s="34">
-        <v>0.99793593583937268</v>
+        <v>0.99793593583937257</v>
       </c>
       <c r="K17" s="92" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L17" s="93">
-        <v>3.2200000000000002E-3</v>
+        <v>2.0600000000000002E-3</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
@@ -10333,20 +10337,20 @@
       </c>
       <c r="G18" s="40">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H18" s="39">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42368</v>
+        <v>42390</v>
       </c>
       <c r="I18" s="34">
         <v>0.9935872951960657</v>
       </c>
       <c r="K18" s="92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L18" s="93">
-        <v>4.8000000000000004E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
@@ -10363,20 +10367,20 @@
       </c>
       <c r="G19" s="40">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H19" s="39">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42734</v>
+        <v>42758</v>
       </c>
       <c r="I19" s="34">
-        <v>0.9857092839281747</v>
+        <v>0.98568312460958118</v>
       </c>
       <c r="K19" s="92" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L19" s="93">
-        <v>6.9500000000000004E-3</v>
+        <v>3.9699999999999996E-3</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
@@ -10393,20 +10397,20 @@
       </c>
       <c r="G20" s="40">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H20" s="39">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43098</v>
+        <v>43122</v>
       </c>
       <c r="I20" s="34">
-        <v>0.97256766471034839</v>
+        <v>0.9725300489006512</v>
       </c>
       <c r="K20" s="92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L20" s="93">
-        <v>9.2100000000000012E-3</v>
+        <v>6.0600000000000003E-3</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
@@ -10423,20 +10427,20 @@
       </c>
       <c r="G21" s="40">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H21" s="39">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43465</v>
+        <v>43486</v>
       </c>
       <c r="I21" s="34">
-        <v>0.95480461717420484</v>
+        <v>0.9548278374505984</v>
       </c>
       <c r="K21" s="92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" s="93">
-        <v>1.1209999999999999E-2</v>
+        <v>8.3000000000000001E-3</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
@@ -10453,20 +10457,20 @@
       </c>
       <c r="G22" s="40">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H22" s="39">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43829</v>
+        <v>43851</v>
       </c>
       <c r="I22" s="34">
-        <v>0.93457206672360638</v>
+        <v>0.93459999143648598</v>
       </c>
       <c r="K22" s="92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L22" s="93">
-        <v>1.2999999999999998E-2</v>
+        <v>1.0489999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
@@ -10483,20 +10487,20 @@
       </c>
       <c r="G23" s="40">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H23" s="39">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44195</v>
+        <v>44217</v>
       </c>
       <c r="I23" s="34">
-        <v>0.91219828545047377</v>
+        <v>0.91223028210710133</v>
       </c>
       <c r="K23" s="92" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L23" s="93">
-        <v>1.4599999999999998E-2</v>
+        <v>1.2540000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
@@ -10513,20 +10517,20 @@
       </c>
       <c r="G24" s="40">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H24" s="39">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44560</v>
+        <v>44582</v>
       </c>
       <c r="I24" s="34">
-        <v>0.88842097435722356</v>
+        <v>0.8884563919667986</v>
       </c>
       <c r="K24" s="92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L24" s="93">
-        <v>1.6080000000000001E-2</v>
+        <v>1.4420000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
@@ -10543,20 +10547,20 @@
       </c>
       <c r="G25" s="40">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H25" s="39">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44925</v>
+        <v>44949</v>
       </c>
       <c r="I25" s="34">
-        <v>0.86331320460478167</v>
+        <v>0.86327571928520708</v>
       </c>
       <c r="K25" s="92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L25" s="93">
-        <v>1.7440000000000001E-2</v>
+        <v>1.609E-2</v>
       </c>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
@@ -10573,20 +10577,20 @@
       </c>
       <c r="G26" s="40">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H26" s="39">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>45289</v>
+        <v>45313</v>
       </c>
       <c r="I26" s="34">
-        <v>0.83719368419591289</v>
+        <v>0.8371537211247585</v>
       </c>
       <c r="K26" s="92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L26" s="93">
-        <v>1.9650000000000001E-2</v>
+        <v>1.7579999999999998E-2</v>
       </c>
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
@@ -10603,20 +10607,20 @@
       </c>
       <c r="G27" s="40">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H27" s="39">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>46021</v>
+        <v>46043</v>
       </c>
       <c r="I27" s="34">
-        <v>0.78505424843857163</v>
+        <v>0.78509555044220203</v>
       </c>
       <c r="K27" s="92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L27" s="93">
-        <v>2.181E-2</v>
+        <v>2.002E-2</v>
       </c>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
@@ -10633,20 +10637,20 @@
       </c>
       <c r="G28" s="40">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H28" s="39">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>47116</v>
+        <v>47140</v>
       </c>
       <c r="I28" s="34">
-        <v>0.71328580373613826</v>
+        <v>0.71324393501997863</v>
       </c>
       <c r="K28" s="92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L28" s="93">
-        <v>2.317E-2</v>
+        <v>2.2540000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
@@ -10663,20 +10667,20 @@
       </c>
       <c r="G29" s="40">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H29" s="39">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>48943</v>
+        <v>48967</v>
       </c>
       <c r="I29" s="34">
-        <v>0.61947121272969474</v>
+        <v>0.61947098304385384</v>
       </c>
       <c r="K29" s="92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L29" s="93">
-        <v>2.3479999999999997E-2</v>
+        <v>2.4379999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
@@ -10693,20 +10697,20 @@
       </c>
       <c r="G30" s="40">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H30" s="39">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>50769</v>
+        <v>50791</v>
       </c>
       <c r="I30" s="34">
-        <v>0.54688184486415126</v>
+        <v>0.54698620920961916</v>
       </c>
       <c r="K30" s="92" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L30" s="93">
-        <v>2.3529999999999999E-2</v>
+        <v>2.4979999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
@@ -10723,20 +10727,20 @@
       </c>
       <c r="G31" s="40">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H31" s="39">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>52595</v>
+        <v>52617</v>
       </c>
       <c r="I31" s="34">
-        <v>0.48614009216505027</v>
+        <v>0.48623249783379141</v>
       </c>
       <c r="K31" s="92" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L31" s="93">
-        <v>2.3768000000000001E-2</v>
+        <v>2.513E-2</v>
       </c>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.2">
@@ -10753,20 +10757,20 @@
       </c>
       <c r="G32" s="40">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H32" s="39">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>54422</v>
+        <v>54444</v>
       </c>
       <c r="I32" s="34">
-        <v>0.42745032022241597</v>
+        <v>0.42756035601851805</v>
       </c>
       <c r="K32" s="92" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L32" s="93">
-        <v>2.4120000000000003E-2</v>
+        <v>2.5319000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.2">
@@ -10783,20 +10787,20 @@
       </c>
       <c r="G33" s="40">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H33" s="39">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>56248</v>
+        <v>56270</v>
       </c>
       <c r="I33" s="34">
-        <v>0.37143928903445578</v>
+        <v>0.37153831640422724</v>
       </c>
       <c r="K33" s="92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L33" s="93">
-        <v>2.4660000000000001E-2</v>
+        <v>2.5559999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.2">
@@ -10813,20 +10817,20 @@
       </c>
       <c r="G34" s="40">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H34" s="39">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>59901</v>
+        <v>59922</v>
       </c>
       <c r="I34" s="34">
-        <v>0.27856908183644158</v>
+        <v>0.2786875493197104</v>
       </c>
       <c r="K34" s="92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L34" s="93">
-        <v>2.504E-2</v>
+        <v>2.5870000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.2">
@@ -10843,16 +10847,21 @@
       </c>
       <c r="G35" s="40">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41638</v>
+        <v>41660</v>
       </c>
       <c r="H35" s="39">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>63552</v>
+        <v>63576</v>
       </c>
       <c r="I35" s="34">
-        <v>0.20786045634669514</v>
-      </c>
-      <c r="K35" s="43"/>
+        <v>0.20792736615750362</v>
+      </c>
+      <c r="K35" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="L35" s="188">
+        <v>2.6079999999999999E-2</v>
+      </c>
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D36" s="42" t="e">

</xml_diff>

<commit_message>
EURYC1M, 3M - reconcile with R010202 prod
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -1481,7 +1481,7 @@
     <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1876,7 +1876,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2190,7 +2189,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2393,7 +2392,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="87">
-        <v>41662.585138888891</v>
+        <v>41663.44253472222</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="58"/>
@@ -9760,7 +9759,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -10859,7 +10858,7 @@
       <c r="K35" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="L35" s="188">
+      <c r="L35" s="93">
         <v>2.6079999999999999E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enable toggle market data live/static
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2189,7 +2189,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2392,7 +2392,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="87">
-        <v>41663.44253472222</v>
+        <v>41666.619976851849</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="58"/>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="D28" s="63">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.20792736615750362</v>
+        <v>0.1986551706738601</v>
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="58"/>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="F84" s="13">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
-        <v>1.6899999999999999E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="G84" s="13">
         <f>_xll.qlSwapRateHelperSpread($E84,Trigger)</f>
@@ -8207,7 +8207,7 @@
       </c>
       <c r="F133" s="20">
         <f>_xll.qlRateHelperQuoteValue($E133,Trigger)</f>
-        <v>2.0699999999999994E-3</v>
+        <v>1.97E-3</v>
       </c>
       <c r="G133" s="20">
         <f>_xll.qlSwapRateHelperSpread($E133,Trigger)</f>
@@ -8249,7 +8249,7 @@
       </c>
       <c r="F134" s="13">
         <f>_xll.qlRateHelperQuoteValue($E134,Trigger)</f>
-        <v>2.2219999999999996E-3</v>
+        <v>1.7320000000000005E-3</v>
       </c>
       <c r="G134" s="13">
         <f>_xll.qlSwapRateHelperSpread($E134,Trigger)</f>
@@ -8291,7 +8291,7 @@
       </c>
       <c r="F135" s="13">
         <f>_xll.qlRateHelperQuoteValue($E135,Trigger)</f>
-        <v>2.6490000000000003E-3</v>
+        <v>2.0290000000000004E-3</v>
       </c>
       <c r="G135" s="13">
         <f>_xll.qlSwapRateHelperSpread($E135,Trigger)</f>
@@ -8333,7 +8333,7 @@
       </c>
       <c r="F136" s="13">
         <f>_xll.qlRateHelperQuoteValue($E136,Trigger)</f>
-        <v>2.8170000000000005E-3</v>
+        <v>1.9970000000000001E-3</v>
       </c>
       <c r="G136" s="13">
         <f>_xll.qlSwapRateHelperSpread($E136,Trigger)</f>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="F137" s="13">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>3.2200000000000002E-3</v>
+        <v>2.3799999999999997E-3</v>
       </c>
       <c r="G137" s="13">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -8417,7 +8417,7 @@
       </c>
       <c r="F138" s="13">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>4.8000000000000004E-3</v>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="G138" s="13">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -8459,7 +8459,7 @@
       </c>
       <c r="F139" s="13">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>6.9500000000000004E-3</v>
+        <v>6.2099999999999994E-3</v>
       </c>
       <c r="G139" s="13">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -8501,7 +8501,7 @@
       </c>
       <c r="F140" s="13">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>9.2100000000000012E-3</v>
+        <v>8.5600000000000016E-3</v>
       </c>
       <c r="G140" s="13">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -8543,7 +8543,7 @@
       </c>
       <c r="F141" s="13">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>1.12E-2</v>
+        <v>1.0799999999999999E-2</v>
       </c>
       <c r="G141" s="13">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -8585,7 +8585,7 @@
       </c>
       <c r="F142" s="13">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>1.2999999999999998E-2</v>
+        <v>1.286E-2</v>
       </c>
       <c r="G142" s="13">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -8627,7 +8627,7 @@
       </c>
       <c r="F143" s="13">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>1.4599999999999998E-2</v>
+        <v>1.473E-2</v>
       </c>
       <c r="G143" s="13">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -8669,7 +8669,7 @@
       </c>
       <c r="F144" s="13">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>1.6070000000000001E-2</v>
+        <v>1.6410000000000001E-2</v>
       </c>
       <c r="G144" s="13">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="F145" s="13">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>1.7430000000000001E-2</v>
+        <v>1.7899999999999999E-2</v>
       </c>
       <c r="G145" s="13">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -8753,7 +8753,7 @@
       </c>
       <c r="F146" s="13">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>1.8620000000000001E-2</v>
+        <v>1.9189999999999999E-2</v>
       </c>
       <c r="G146" s="13">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -8795,7 +8795,7 @@
       </c>
       <c r="F147" s="13">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>1.9650000000000001E-2</v>
+        <v>2.0320000000000001E-2</v>
       </c>
       <c r="G147" s="13">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -8837,7 +8837,7 @@
       </c>
       <c r="F148" s="13">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>2.0523E-2</v>
+        <v>2.1284999999999998E-2</v>
       </c>
       <c r="G148" s="13">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -8879,7 +8879,7 @@
       </c>
       <c r="F149" s="13">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>2.1239000000000004E-2</v>
+        <v>2.2089999999999999E-2</v>
       </c>
       <c r="G149" s="13">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="F150" s="13">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>2.181E-2</v>
+        <v>2.2750000000000003E-2</v>
       </c>
       <c r="G150" s="13">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="F151" s="13">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>2.2257000000000002E-2</v>
+        <v>2.3285999999999998E-2</v>
       </c>
       <c r="G151" s="13">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -9005,7 +9005,7 @@
       </c>
       <c r="F152" s="13">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>2.2599999999999999E-2</v>
+        <v>2.3710000000000002E-2</v>
       </c>
       <c r="G152" s="13">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -9047,7 +9047,7 @@
       </c>
       <c r="F153" s="13">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>2.2849999999999999E-2</v>
+        <v>2.4040000000000002E-2</v>
       </c>
       <c r="G153" s="13">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -9089,7 +9089,7 @@
       </c>
       <c r="F154" s="13">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>2.3037000000000002E-2</v>
+        <v>2.4306999999999999E-2</v>
       </c>
       <c r="G154" s="13">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="F155" s="13">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>2.317E-2</v>
+        <v>2.4510000000000001E-2</v>
       </c>
       <c r="G155" s="13">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -9173,7 +9173,7 @@
       </c>
       <c r="F156" s="13">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>2.3269999999999999E-2</v>
+        <v>2.4688999999999999E-2</v>
       </c>
       <c r="G156" s="13">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="F157" s="13">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>2.3356000000000002E-2</v>
+        <v>2.4816000000000001E-2</v>
       </c>
       <c r="G157" s="13">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -9257,7 +9257,7 @@
       </c>
       <c r="F158" s="13">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>2.3419999999999996E-2</v>
+        <v>2.4929000000000003E-2</v>
       </c>
       <c r="G158" s="13">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -9299,7 +9299,7 @@
       </c>
       <c r="F159" s="13">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>2.3450999999999996E-2</v>
+        <v>2.5010000000000001E-2</v>
       </c>
       <c r="G159" s="13">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -9341,7 +9341,7 @@
       </c>
       <c r="F160" s="13">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>2.3479999999999997E-2</v>
+        <v>2.5070000000000002E-2</v>
       </c>
       <c r="G160" s="13">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -9383,7 +9383,7 @@
       </c>
       <c r="F161" s="13">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>2.3497000000000001E-2</v>
+        <v>2.5108000000000002E-2</v>
       </c>
       <c r="G161" s="13">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -9425,7 +9425,7 @@
       </c>
       <c r="F162" s="13">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>2.3502000000000002E-2</v>
+        <v>2.5145999999999998E-2</v>
       </c>
       <c r="G162" s="13">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="F163" s="13">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>2.3496E-2</v>
+        <v>2.5162E-2</v>
       </c>
       <c r="G163" s="13">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="F164" s="13">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>2.3508999999999995E-2</v>
+        <v>2.5177000000000001E-2</v>
       </c>
       <c r="G164" s="13">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
@@ -9551,7 +9551,7 @@
       </c>
       <c r="F165" s="13">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>2.3519999999999996E-2</v>
+        <v>2.5200000000000004E-2</v>
       </c>
       <c r="G165" s="13">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -9593,7 +9593,7 @@
       </c>
       <c r="F166" s="13">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>2.3754000000000001E-2</v>
+        <v>2.5378000000000001E-2</v>
       </c>
       <c r="G166" s="13">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -9635,7 +9635,7 @@
       </c>
       <c r="F167" s="13">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>2.4109999999999999E-2</v>
+        <v>2.5610000000000004E-2</v>
       </c>
       <c r="G167" s="13">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -9677,7 +9677,7 @@
       </c>
       <c r="F168" s="13">
         <f>_xll.qlRateHelperQuoteValue($E168,Trigger)</f>
-        <v>2.4660000000000001E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="G168" s="13">
         <f>_xll.qlSwapRateHelperSpread($E168,Trigger)</f>
@@ -9719,7 +9719,7 @@
       </c>
       <c r="F169" s="6">
         <f>_xll.qlRateHelperQuoteValue($E169,Trigger)</f>
-        <v>2.504E-2</v>
+        <v>2.6100000000000005E-2</v>
       </c>
       <c r="G169" s="6">
         <f>_xll.qlSwapRateHelperSpread($E169,Trigger)</f>
@@ -9759,7 +9759,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="E13" s="41">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>1.6899999999999999E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="F13" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10193,7 +10193,7 @@
         <v>41904</v>
       </c>
       <c r="I13" s="34">
-        <v>0.9988558660973782</v>
+        <v>0.99884910386587911</v>
       </c>
       <c r="K13" s="92" t="s">
         <v>126</v>
@@ -10223,7 +10223,7 @@
         <v>41933</v>
       </c>
       <c r="I14" s="34">
-        <v>0.99864442341558202</v>
+        <v>0.99864442341558224</v>
       </c>
       <c r="K14" s="92" t="s">
         <v>127</v>
@@ -10283,7 +10283,7 @@
         <v>41995</v>
       </c>
       <c r="I16" s="34">
-        <v>0.99818870341526134</v>
+        <v>0.99818870341526145</v>
       </c>
       <c r="K16" s="92" t="s">
         <v>129</v>
@@ -10313,7 +10313,7 @@
         <v>42025</v>
       </c>
       <c r="I17" s="34">
-        <v>0.99793593583937257</v>
+        <v>0.99793593583937268</v>
       </c>
       <c r="K17" s="92" t="s">
         <v>130</v>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="E18" s="41">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>3.2200000000000002E-3</v>
+        <v>2.3799999999999997E-3</v>
       </c>
       <c r="F18" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10343,7 +10343,7 @@
         <v>42390</v>
       </c>
       <c r="I18" s="34">
-        <v>0.9935872951960657</v>
+        <v>0.99525620271025184</v>
       </c>
       <c r="K18" s="92" t="s">
         <v>131</v>
@@ -10358,7 +10358,7 @@
       </c>
       <c r="E19" s="41">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>4.8000000000000004E-3</v>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="F19" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10373,7 +10373,7 @@
         <v>42758</v>
       </c>
       <c r="I19" s="34">
-        <v>0.98568312460958118</v>
+        <v>0.98820180836998395</v>
       </c>
       <c r="K19" s="92" t="s">
         <v>132</v>
@@ -10388,7 +10388,7 @@
       </c>
       <c r="E20" s="41">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>6.9500000000000004E-3</v>
+        <v>6.2099999999999994E-3</v>
       </c>
       <c r="F20" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10403,7 +10403,7 @@
         <v>43122</v>
       </c>
       <c r="I20" s="34">
-        <v>0.9725300489006512</v>
+        <v>0.97541097431604573</v>
       </c>
       <c r="K20" s="92" t="s">
         <v>133</v>
@@ -10418,7 +10418,7 @@
       </c>
       <c r="E21" s="41">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>9.2100000000000012E-3</v>
+        <v>8.5600000000000016E-3</v>
       </c>
       <c r="F21" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10433,7 +10433,7 @@
         <v>43486</v>
       </c>
       <c r="I21" s="34">
-        <v>0.9548278374505984</v>
+        <v>0.95792885491498059</v>
       </c>
       <c r="K21" s="92" t="s">
         <v>134</v>
@@ -10448,7 +10448,7 @@
       </c>
       <c r="E22" s="41">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.12E-2</v>
+        <v>1.0799999999999999E-2</v>
       </c>
       <c r="F22" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10463,7 +10463,7 @@
         <v>43851</v>
       </c>
       <c r="I22" s="34">
-        <v>0.93459999143648598</v>
+        <v>0.93680212040358968</v>
       </c>
       <c r="K22" s="92" t="s">
         <v>135</v>
@@ -10478,7 +10478,7 @@
       </c>
       <c r="E23" s="41">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.2999999999999998E-2</v>
+        <v>1.286E-2</v>
       </c>
       <c r="F23" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10493,7 +10493,7 @@
         <v>44217</v>
       </c>
       <c r="I23" s="34">
-        <v>0.91223028210710133</v>
+        <v>0.91300644712608492</v>
       </c>
       <c r="K23" s="92" t="s">
         <v>136</v>
@@ -10508,7 +10508,7 @@
       </c>
       <c r="E24" s="41">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.4599999999999998E-2</v>
+        <v>1.473E-2</v>
       </c>
       <c r="F24" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10523,7 +10523,7 @@
         <v>44582</v>
       </c>
       <c r="I24" s="34">
-        <v>0.8884563919667986</v>
+        <v>0.88728679476407535</v>
       </c>
       <c r="K24" s="92" t="s">
         <v>137</v>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="E25" s="41">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>1.6070000000000001E-2</v>
+        <v>1.6410000000000001E-2</v>
       </c>
       <c r="F25" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10553,7 +10553,7 @@
         <v>44949</v>
       </c>
       <c r="I25" s="34">
-        <v>0.86327571928520708</v>
+        <v>0.86023661312126376</v>
       </c>
       <c r="K25" s="92" t="s">
         <v>138</v>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="E26" s="41">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>1.7430000000000001E-2</v>
+        <v>1.7899999999999999E-2</v>
       </c>
       <c r="F26" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10583,7 +10583,7 @@
         <v>45313</v>
       </c>
       <c r="I26" s="34">
-        <v>0.8371537211247585</v>
+        <v>0.83268271824623075</v>
       </c>
       <c r="K26" s="92" t="s">
         <v>139</v>
@@ -10598,7 +10598,7 @@
       </c>
       <c r="E27" s="41">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>1.9650000000000001E-2</v>
+        <v>2.0320000000000001E-2</v>
       </c>
       <c r="F27" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10613,7 +10613,7 @@
         <v>46043</v>
       </c>
       <c r="I27" s="34">
-        <v>0.78509555044220203</v>
+        <v>0.77794038782040686</v>
       </c>
       <c r="K27" s="92" t="s">
         <v>140</v>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="E28" s="41">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.181E-2</v>
+        <v>2.2750000000000003E-2</v>
       </c>
       <c r="F28" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10643,7 +10643,7 @@
         <v>47140</v>
       </c>
       <c r="I28" s="34">
-        <v>0.71324393501997863</v>
+        <v>0.70176144096658721</v>
       </c>
       <c r="K28" s="92" t="s">
         <v>141</v>
@@ -10658,7 +10658,7 @@
       </c>
       <c r="E29" s="41">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.317E-2</v>
+        <v>2.4510000000000001E-2</v>
       </c>
       <c r="F29" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10673,7 +10673,7 @@
         <v>48967</v>
       </c>
       <c r="I29" s="34">
-        <v>0.61947098304385384</v>
+        <v>0.60038133735263344</v>
       </c>
       <c r="K29" s="92" t="s">
         <v>142</v>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="E30" s="41">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.3479999999999997E-2</v>
+        <v>2.5070000000000002E-2</v>
       </c>
       <c r="F30" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -10703,7 +10703,7 @@
         <v>50791</v>
       </c>
       <c r="I30" s="34">
-        <v>0.54698620920961916</v>
+        <v>0.52214294545702122</v>
       </c>
       <c r="K30" s="92" t="s">
         <v>143</v>
@@ -10718,7 +10718,7 @@
       </c>
       <c r="E31" s="41">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.3519999999999996E-2</v>
+        <v>2.5200000000000004E-2</v>
       </c>
       <c r="F31" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -10733,7 +10733,7 @@
         <v>52617</v>
       </c>
       <c r="I31" s="34">
-        <v>0.48623249783379141</v>
+        <v>0.45876435150840095</v>
       </c>
       <c r="K31" s="92" t="s">
         <v>144</v>
@@ -10748,7 +10748,7 @@
       </c>
       <c r="E32" s="41">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.3754000000000001E-2</v>
+        <v>2.5378000000000001E-2</v>
       </c>
       <c r="F32" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -10763,7 +10763,7 @@
         <v>54444</v>
       </c>
       <c r="I32" s="34">
-        <v>0.42756035601851805</v>
+        <v>0.40115551498927415</v>
       </c>
       <c r="K32" s="92" t="s">
         <v>145</v>
@@ -10778,7 +10778,7 @@
       </c>
       <c r="E33" s="41">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.4109999999999999E-2</v>
+        <v>2.5610000000000004E-2</v>
       </c>
       <c r="F33" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -10793,7 +10793,7 @@
         <v>56270</v>
       </c>
       <c r="I33" s="34">
-        <v>0.37153831640422724</v>
+        <v>0.34842834944111811</v>
       </c>
       <c r="K33" s="92" t="s">
         <v>146</v>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="E34" s="41">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.4660000000000001E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="F34" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -10823,7 +10823,7 @@
         <v>59922</v>
       </c>
       <c r="I34" s="34">
-        <v>0.2786875493197104</v>
+        <v>0.26344063375472976</v>
       </c>
       <c r="K34" s="92" t="s">
         <v>147</v>
@@ -10838,7 +10838,7 @@
       </c>
       <c r="E35" s="41">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.504E-2</v>
+        <v>2.6100000000000005E-2</v>
       </c>
       <c r="F35" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -10853,7 +10853,7 @@
         <v>63576</v>
       </c>
       <c r="I35" s="34">
-        <v>0.20792736615750362</v>
+        <v>0.1986551706738601</v>
       </c>
       <c r="K35" s="43" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
use the same formatting for all of the General Settings worksheets
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -953,7 +953,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1010,12 +1010,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1422,15 +1428,11 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1439,31 +1441,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1814,8 +1794,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1831,19 +1811,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="13" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1851,16 +1823,21 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1875,6 +1852,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2193,26 +2173,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="166" customWidth="1"/>
-    <col min="3" max="3" width="18" style="166" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="166" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="166" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.7109375" style="166" customWidth="1"/>
-    <col min="8" max="9" width="8" style="166"/>
-    <col min="10" max="11" width="2.7109375" style="166" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="166" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.7109375" style="166" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="166" customWidth="1"/>
-    <col min="15" max="16384" width="8" style="166"/>
+    <col min="1" max="2" width="2.7109375" style="171" customWidth="1"/>
+    <col min="3" max="3" width="18" style="171" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="171" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="171" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.7109375" style="171" customWidth="1"/>
+    <col min="8" max="8" width="4" style="171" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="171" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" style="171" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="171" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.7109375" style="171" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="171" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="171"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="166" t="str">
+      <c r="B1" s="171" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Dec  5 2013 11:03:51</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Feb  7 2014 15:33:58</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="179" t="s">
         <v>115</v>
       </c>
@@ -2225,7 +2206,7 @@
       </c>
       <c r="L2" s="180"/>
       <c r="M2" s="180"/>
-      <c r="N2" s="182"/>
+      <c r="N2" s="187"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
@@ -2248,10 +2229,10 @@
       </c>
       <c r="E4" s="59"/>
       <c r="F4" s="58"/>
-      <c r="H4" s="169" t="s">
+      <c r="H4" s="173" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="170"/>
+      <c r="I4" s="174"/>
       <c r="K4" s="129"/>
       <c r="L4" s="128" t="s">
         <v>163</v>
@@ -2271,10 +2252,10 @@
       </c>
       <c r="E5" s="59"/>
       <c r="F5" s="58"/>
-      <c r="H5" s="167" t="s">
+      <c r="H5" s="175" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="168" t="s">
+      <c r="I5" s="176" t="s">
         <v>110</v>
       </c>
       <c r="K5" s="129"/>
@@ -2283,7 +2264,7 @@
       </c>
       <c r="M5" s="130" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data2\XML\</v>
+        <v>C:\Users\erik\Documents\repos\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="N5" s="127"/>
     </row>
@@ -2298,10 +2279,10 @@
       </c>
       <c r="E6" s="59"/>
       <c r="F6" s="58"/>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="175" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="168"/>
+      <c r="I6" s="176"/>
       <c r="K6" s="129"/>
       <c r="L6" s="128" t="s">
         <v>161</v>
@@ -2322,10 +2303,10 @@
       </c>
       <c r="E7" s="59"/>
       <c r="F7" s="58"/>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="168"/>
+      <c r="I7" s="176"/>
       <c r="K7" s="126"/>
       <c r="L7" s="125"/>
       <c r="M7" s="125"/>
@@ -2342,18 +2323,18 @@
       </c>
       <c r="E8" s="59"/>
       <c r="F8" s="58"/>
-      <c r="H8" s="171" t="s">
+      <c r="H8" s="177" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="172" t="s">
+      <c r="I8" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="173"/>
-      <c r="L8" s="173"/>
-      <c r="M8" s="173"/>
-      <c r="N8" s="173"/>
-    </row>
-    <row r="9" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="K8" s="172"/>
+      <c r="L8" s="172"/>
+      <c r="M8" s="172"/>
+      <c r="N8" s="172"/>
+    </row>
+    <row r="9" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="62"/>
       <c r="C9" s="89" t="s">
         <v>102</v>
@@ -2369,7 +2350,7 @@
       </c>
       <c r="L9" s="180"/>
       <c r="M9" s="180"/>
-      <c r="N9" s="182"/>
+      <c r="N9" s="187"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="62"/>
@@ -2392,7 +2373,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="87">
-        <v>41666.619976851849</v>
+        <v>41684.584456018521</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="58"/>
@@ -2470,18 +2451,18 @@
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
-      <c r="E15" s="178" t="s">
+      <c r="E15" s="170" t="s">
         <v>197</v>
       </c>
       <c r="F15" s="58"/>
-      <c r="K15" s="174"/>
-      <c r="L15" s="175" t="s">
+      <c r="K15" s="166"/>
+      <c r="L15" s="167" t="s">
         <v>193</v>
       </c>
-      <c r="M15" s="176" t="s">
+      <c r="M15" s="168" t="s">
         <v>194</v>
       </c>
-      <c r="N15" s="177"/>
+      <c r="N15" s="169"/>
     </row>
     <row r="16" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="62"/>
@@ -2494,14 +2475,14 @@
       </c>
       <c r="E16" s="59"/>
       <c r="F16" s="58"/>
-      <c r="K16" s="174"/>
-      <c r="L16" s="175" t="s">
+      <c r="K16" s="166"/>
+      <c r="L16" s="167" t="s">
         <v>195</v>
       </c>
-      <c r="M16" s="176" t="s">
+      <c r="M16" s="168" t="s">
         <v>196</v>
       </c>
-      <c r="N16" s="177"/>
+      <c r="N16" s="169"/>
     </row>
     <row r="17" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="62"/>
@@ -2628,7 +2609,7 @@
       <c r="B27" s="62"/>
       <c r="C27" s="66">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="D27" s="65">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2641,11 +2622,11 @@
       <c r="B28" s="62"/>
       <c r="C28" s="64">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>63576</v>
+        <v>63604</v>
       </c>
       <c r="D28" s="63">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.1986551706738601</v>
+        <v>0.19865517067371108</v>
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="58"/>
@@ -2738,11 +2719,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="183" t="s">
+      <c r="B1" s="182" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="184"/>
-      <c r="D1" s="185"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="184"/>
       <c r="E1" s="31" t="s">
         <v>74</v>
       </c>
@@ -2872,11 +2853,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41661</v>
+        <v>41689</v>
       </c>
       <c r="M4" s="1">
         <v>30</v>
@@ -2911,11 +2892,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41667</v>
+        <v>41695</v>
       </c>
       <c r="M5" s="1">
         <v>40</v>
@@ -2950,11 +2931,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41674</v>
+        <v>41702</v>
       </c>
       <c r="M6" s="1">
         <v>50</v>
@@ -2989,11 +2970,11 @@
       </c>
       <c r="K7" s="11">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L7" s="10">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41681</v>
+        <v>41709</v>
       </c>
       <c r="M7" s="1">
         <v>60</v>
@@ -3028,11 +3009,11 @@
       </c>
       <c r="K8" s="11">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L8" s="10">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41691</v>
+        <v>41716</v>
       </c>
       <c r="M8" s="1">
         <v>70</v>
@@ -5832,11 +5813,11 @@
       </c>
       <c r="K78" s="18">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L78" s="17">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>41719</v>
+        <v>41751</v>
       </c>
       <c r="M78" s="22"/>
     </row>
@@ -5871,11 +5852,11 @@
       </c>
       <c r="K79" s="11">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L79" s="10">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>41751</v>
+        <v>41778</v>
       </c>
       <c r="M79" s="25"/>
     </row>
@@ -5910,11 +5891,11 @@
       </c>
       <c r="K80" s="11">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L80" s="10">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>41780</v>
+        <v>41808</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
@@ -5948,11 +5929,11 @@
       </c>
       <c r="K81" s="11">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L81" s="10">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>41813</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="82" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5986,11 +5967,11 @@
       </c>
       <c r="K82" s="11">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L82" s="10">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>41841</v>
+        <v>41869</v>
       </c>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.2">
@@ -6024,11 +6005,11 @@
       </c>
       <c r="K83" s="11">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L83" s="10">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>41872</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
@@ -6062,11 +6043,11 @@
       </c>
       <c r="K84" s="11">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L84" s="10">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>41904</v>
+        <v>41932</v>
       </c>
     </row>
     <row r="85" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6100,11 +6081,11 @@
       </c>
       <c r="K85" s="11">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L85" s="10">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>41933</v>
+        <v>41961</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
@@ -6138,11 +6119,11 @@
       </c>
       <c r="K86" s="11">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L86" s="10">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>41964</v>
+        <v>41991</v>
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
@@ -6176,11 +6157,11 @@
       </c>
       <c r="K87" s="11">
         <f>_xll.qlRateHelperEarliestDate($E87,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L87" s="10">
         <f>_xll.qlRateHelperLatestDate($E87,Trigger)</f>
-        <v>41995</v>
+        <v>42023</v>
       </c>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.2">
@@ -6214,11 +6195,11 @@
       </c>
       <c r="K88" s="4">
         <f>_xll.qlRateHelperEarliestDate($E88,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L88" s="3">
         <f>_xll.qlRateHelperLatestDate($E88,Trigger)</f>
-        <v>42025</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="89" spans="2:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8224,11 +8205,11 @@
       </c>
       <c r="K133" s="18">
         <f>_xll.qlRateHelperEarliestDate($E133,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L133" s="17">
         <f>_xll.qlRateHelperLatestDate($E133,Trigger)</f>
-        <v>42025</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.2">
@@ -8266,11 +8247,11 @@
       </c>
       <c r="K134" s="11">
         <f>_xll.qlRateHelperEarliestDate($E134,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L134" s="10">
         <f>_xll.qlRateHelperLatestDate($E134,Trigger)</f>
-        <v>42115</v>
+        <v>42142</v>
       </c>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.2">
@@ -8308,11 +8289,11 @@
       </c>
       <c r="K135" s="11">
         <f>_xll.qlRateHelperEarliestDate($E135,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L135" s="10">
         <f>_xll.qlRateHelperLatestDate($E135,Trigger)</f>
-        <v>42206</v>
+        <v>42234</v>
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.2">
@@ -8350,11 +8331,11 @@
       </c>
       <c r="K136" s="11">
         <f>_xll.qlRateHelperEarliestDate($E136,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L136" s="10">
         <f>_xll.qlRateHelperLatestDate($E136,Trigger)</f>
-        <v>42298</v>
+        <v>42326</v>
       </c>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.2">
@@ -8392,11 +8373,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>42390</v>
+        <v>42418</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8434,11 +8415,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>42758</v>
+        <v>42786</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8476,11 +8457,11 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>43122</v>
+        <v>43150</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
@@ -8518,11 +8499,11 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>43486</v>
+        <v>43514</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
@@ -8560,11 +8541,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>43851</v>
+        <v>43879</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8602,11 +8583,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>44217</v>
+        <v>44245</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8644,11 +8625,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>44582</v>
+        <v>44610</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8686,11 +8667,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>44949</v>
+        <v>44977</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8728,11 +8709,11 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>45313</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
@@ -8770,11 +8751,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>45678</v>
+        <v>45706</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8812,11 +8793,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46043</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8854,11 +8835,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>46408</v>
+        <v>46436</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8896,11 +8877,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>46773</v>
+        <v>46801</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8938,11 +8919,11 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>47140</v>
+        <v>47168</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
@@ -8980,11 +8961,11 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>47504</v>
+        <v>47532</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
@@ -9022,11 +9003,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>47869</v>
+        <v>47897</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -9064,11 +9045,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>48234</v>
+        <v>48262</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -9106,11 +9087,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>48600</v>
+        <v>48628</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9148,11 +9129,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>48967</v>
+        <v>48995</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9190,11 +9171,11 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>49331</v>
+        <v>49359</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
@@ -9232,11 +9213,11 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>49695</v>
+        <v>49723</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
@@ -9274,11 +9255,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50061</v>
+        <v>50089</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9316,11 +9297,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>50426</v>
+        <v>50454</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9358,11 +9339,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>50791</v>
+        <v>50819</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9400,11 +9381,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>51158</v>
+        <v>51186</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9442,11 +9423,11 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>51522</v>
+        <v>51550</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.2">
@@ -9484,11 +9465,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>51887</v>
+        <v>51915</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9526,11 +9507,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>52252</v>
+        <v>52280</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9568,11 +9549,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>52617</v>
+        <v>52645</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9610,11 +9591,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>54444</v>
+        <v>54472</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9652,11 +9633,11 @@
       </c>
       <c r="K167" s="11">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L167" s="10">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>56270</v>
+        <v>56298</v>
       </c>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.2">
@@ -9694,11 +9675,11 @@
       </c>
       <c r="K168" s="11">
         <f>_xll.qlRateHelperEarliestDate($E168,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L168" s="10">
         <f>_xll.qlRateHelperLatestDate($E168,Trigger)</f>
-        <v>59922</v>
+        <v>59950</v>
       </c>
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.2">
@@ -9736,11 +9717,11 @@
       </c>
       <c r="K169" s="4">
         <f>_xll.qlRateHelperEarliestDate($E169,Trigger)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="L169" s="3">
         <f>_xll.qlRateHelperLatestDate($E169,Trigger)</f>
-        <v>63576</v>
+        <v>63604</v>
       </c>
     </row>
   </sheetData>
@@ -9780,10 +9761,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="187"/>
+      <c r="B1" s="186"/>
       <c r="D1" s="54" t="s">
         <v>83</v>
       </c>
@@ -9823,11 +9804,11 @@
       </c>
       <c r="G2" s="40">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H2" s="39">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41661</v>
+        <v>41689</v>
       </c>
       <c r="I2" s="34">
         <v>0.99999652778983417</v>
@@ -9859,11 +9840,11 @@
       </c>
       <c r="G3" s="40">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H3" s="39">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41667</v>
+        <v>41695</v>
       </c>
       <c r="I3" s="34">
         <v>0.99997413955766812</v>
@@ -9895,11 +9876,11 @@
       </c>
       <c r="G4" s="40">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H4" s="39">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41674</v>
+        <v>41702</v>
       </c>
       <c r="I4" s="34">
         <v>0.99994905815077162</v>
@@ -9931,11 +9912,11 @@
       </c>
       <c r="G5" s="40">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H5" s="39">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41681</v>
+        <v>41709</v>
       </c>
       <c r="I5" s="34">
         <v>0.99992358917239399</v>
@@ -9968,14 +9949,14 @@
       </c>
       <c r="G6" s="40">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H6" s="39">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41691</v>
+        <v>41716</v>
       </c>
       <c r="I6" s="34">
-        <v>0.99988720716810242</v>
+        <v>0.99989812149139912</v>
       </c>
       <c r="K6" s="92" t="s">
         <v>119</v>
@@ -10006,14 +9987,14 @@
       </c>
       <c r="G7" s="40">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H7" s="39">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41719</v>
+        <v>41751</v>
       </c>
       <c r="I7" s="34">
-        <v>0.99977716077963408</v>
+        <v>0.99976205663052187</v>
       </c>
       <c r="K7" s="92" t="s">
         <v>120</v>
@@ -10036,14 +10017,14 @@
       </c>
       <c r="G8" s="40">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H8" s="39">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41751</v>
+        <v>41778</v>
       </c>
       <c r="I8" s="34">
-        <v>0.99964118435043958</v>
+        <v>0.99964512598027699</v>
       </c>
       <c r="K8" s="92" t="s">
         <v>121</v>
@@ -10066,14 +10047,14 @@
       </c>
       <c r="G9" s="40">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H9" s="39">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41780</v>
+        <v>41808</v>
       </c>
       <c r="I9" s="34">
-        <v>0.99951357006256958</v>
+        <v>0.99951357006256947</v>
       </c>
       <c r="K9" s="92" t="s">
         <v>122</v>
@@ -10096,14 +10077,14 @@
       </c>
       <c r="G10" s="40">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41813</v>
+        <v>41838</v>
       </c>
       <c r="I10" s="34">
-        <v>0.99935866157893161</v>
+        <v>0.9993712289351282</v>
       </c>
       <c r="K10" s="92" t="s">
         <v>123</v>
@@ -10126,14 +10107,14 @@
       </c>
       <c r="G11" s="40">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41841</v>
+        <v>41869</v>
       </c>
       <c r="I11" s="34">
-        <v>0.99920624166391381</v>
+        <v>0.9992062416639137</v>
       </c>
       <c r="K11" s="92" t="s">
         <v>124</v>
@@ -10156,14 +10137,14 @@
       </c>
       <c r="G12" s="40">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41872</v>
+        <v>41900</v>
       </c>
       <c r="I12" s="34">
-        <v>0.99904103161420954</v>
+        <v>0.99904103161420921</v>
       </c>
       <c r="K12" s="92" t="s">
         <v>125</v>
@@ -10186,14 +10167,14 @@
       </c>
       <c r="G13" s="40">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>41904</v>
+        <v>41932</v>
       </c>
       <c r="I13" s="34">
-        <v>0.99884910386587911</v>
+        <v>0.99884910386587877</v>
       </c>
       <c r="K13" s="92" t="s">
         <v>126</v>
@@ -10216,14 +10197,14 @@
       </c>
       <c r="G14" s="40">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>41933</v>
+        <v>41961</v>
       </c>
       <c r="I14" s="34">
-        <v>0.99864442341558224</v>
+        <v>0.99864442341558191</v>
       </c>
       <c r="K14" s="92" t="s">
         <v>127</v>
@@ -10246,14 +10227,14 @@
       </c>
       <c r="G15" s="40">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>41964</v>
+        <v>41991</v>
       </c>
       <c r="I15" s="34">
-        <v>0.99843179645836277</v>
+        <v>0.99843694695953467</v>
       </c>
       <c r="K15" s="92" t="s">
         <v>128</v>
@@ -10276,14 +10257,14 @@
       </c>
       <c r="G16" s="40">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>41995</v>
+        <v>42023</v>
       </c>
       <c r="I16" s="34">
-        <v>0.99818870341526145</v>
+        <v>0.99818870341526122</v>
       </c>
       <c r="K16" s="92" t="s">
         <v>129</v>
@@ -10306,14 +10287,14 @@
       </c>
       <c r="G17" s="40">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H17" s="39">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42025</v>
+        <v>42053</v>
       </c>
       <c r="I17" s="34">
-        <v>0.99793593583937268</v>
+        <v>0.99793593583937223</v>
       </c>
       <c r="K17" s="92" t="s">
         <v>130</v>
@@ -10336,14 +10317,14 @@
       </c>
       <c r="G18" s="40">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H18" s="39">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42390</v>
+        <v>42418</v>
       </c>
       <c r="I18" s="34">
-        <v>0.99525620271025184</v>
+        <v>0.99525620271025161</v>
       </c>
       <c r="K18" s="92" t="s">
         <v>131</v>
@@ -10366,14 +10347,14 @@
       </c>
       <c r="G19" s="40">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H19" s="39">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42758</v>
+        <v>42786</v>
       </c>
       <c r="I19" s="34">
-        <v>0.98820180836998395</v>
+        <v>0.98820180836998406</v>
       </c>
       <c r="K19" s="92" t="s">
         <v>132</v>
@@ -10396,14 +10377,14 @@
       </c>
       <c r="G20" s="40">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H20" s="39">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43122</v>
+        <v>43150</v>
       </c>
       <c r="I20" s="34">
-        <v>0.97541097431604573</v>
+        <v>0.97541097431604429</v>
       </c>
       <c r="K20" s="92" t="s">
         <v>133</v>
@@ -10426,14 +10407,14 @@
       </c>
       <c r="G21" s="40">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H21" s="39">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43486</v>
+        <v>43514</v>
       </c>
       <c r="I21" s="34">
-        <v>0.95792885491498059</v>
+        <v>0.95792885491498114</v>
       </c>
       <c r="K21" s="92" t="s">
         <v>134</v>
@@ -10456,14 +10437,14 @@
       </c>
       <c r="G22" s="40">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H22" s="39">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43851</v>
+        <v>43879</v>
       </c>
       <c r="I22" s="34">
-        <v>0.93680212040358968</v>
+        <v>0.93680212040358812</v>
       </c>
       <c r="K22" s="92" t="s">
         <v>135</v>
@@ -10486,14 +10467,14 @@
       </c>
       <c r="G23" s="40">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H23" s="39">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44217</v>
+        <v>44245</v>
       </c>
       <c r="I23" s="34">
-        <v>0.91300644712608492</v>
+        <v>0.91300644712608425</v>
       </c>
       <c r="K23" s="92" t="s">
         <v>136</v>
@@ -10516,14 +10497,14 @@
       </c>
       <c r="G24" s="40">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H24" s="39">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44582</v>
+        <v>44610</v>
       </c>
       <c r="I24" s="34">
-        <v>0.88728679476407535</v>
+        <v>0.88728679476407502</v>
       </c>
       <c r="K24" s="92" t="s">
         <v>137</v>
@@ -10546,14 +10527,14 @@
       </c>
       <c r="G25" s="40">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H25" s="39">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44949</v>
+        <v>44977</v>
       </c>
       <c r="I25" s="34">
-        <v>0.86023661312126376</v>
+        <v>0.86023661312126487</v>
       </c>
       <c r="K25" s="92" t="s">
         <v>138</v>
@@ -10576,14 +10557,14 @@
       </c>
       <c r="G26" s="40">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H26" s="39">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>45313</v>
+        <v>45341</v>
       </c>
       <c r="I26" s="34">
-        <v>0.83268271824623075</v>
+        <v>0.83268271824622997</v>
       </c>
       <c r="K26" s="92" t="s">
         <v>139</v>
@@ -10606,14 +10587,14 @@
       </c>
       <c r="G27" s="40">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H27" s="39">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>46043</v>
+        <v>46071</v>
       </c>
       <c r="I27" s="34">
-        <v>0.77794038782040686</v>
+        <v>0.77794038781990571</v>
       </c>
       <c r="K27" s="92" t="s">
         <v>140</v>
@@ -10636,14 +10617,14 @@
       </c>
       <c r="G28" s="40">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H28" s="39">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>47140</v>
+        <v>47168</v>
       </c>
       <c r="I28" s="34">
-        <v>0.70176144096658721</v>
+        <v>0.70176144096650395</v>
       </c>
       <c r="K28" s="92" t="s">
         <v>141</v>
@@ -10666,14 +10647,14 @@
       </c>
       <c r="G29" s="40">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H29" s="39">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>48967</v>
+        <v>48995</v>
       </c>
       <c r="I29" s="34">
-        <v>0.60038133735263344</v>
+        <v>0.60038133735216315</v>
       </c>
       <c r="K29" s="92" t="s">
         <v>142</v>
@@ -10696,14 +10677,14 @@
       </c>
       <c r="G30" s="40">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H30" s="39">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>50791</v>
+        <v>50819</v>
       </c>
       <c r="I30" s="34">
-        <v>0.52214294545702122</v>
+        <v>0.52214294545669226</v>
       </c>
       <c r="K30" s="92" t="s">
         <v>143</v>
@@ -10726,14 +10707,14 @@
       </c>
       <c r="G31" s="40">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H31" s="39">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>52617</v>
+        <v>52645</v>
       </c>
       <c r="I31" s="34">
-        <v>0.45876435150840095</v>
+        <v>0.45876435150808414</v>
       </c>
       <c r="K31" s="92" t="s">
         <v>144</v>
@@ -10756,14 +10737,14 @@
       </c>
       <c r="G32" s="40">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H32" s="39">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>54444</v>
+        <v>54472</v>
       </c>
       <c r="I32" s="34">
-        <v>0.40115551498927415</v>
+        <v>0.40115551498899932</v>
       </c>
       <c r="K32" s="92" t="s">
         <v>145</v>
@@ -10786,14 +10767,14 @@
       </c>
       <c r="G33" s="40">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H33" s="39">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>56270</v>
+        <v>56298</v>
       </c>
       <c r="I33" s="34">
-        <v>0.34842834944111811</v>
+        <v>0.34842834944087098</v>
       </c>
       <c r="K33" s="92" t="s">
         <v>146</v>
@@ -10816,14 +10797,14 @@
       </c>
       <c r="G34" s="40">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H34" s="39">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>59922</v>
+        <v>59950</v>
       </c>
       <c r="I34" s="34">
-        <v>0.26344063375472976</v>
+        <v>0.26344063375453741</v>
       </c>
       <c r="K34" s="92" t="s">
         <v>147</v>
@@ -10846,14 +10827,14 @@
       </c>
       <c r="G35" s="40">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41660</v>
+        <v>41688</v>
       </c>
       <c r="H35" s="39">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>63576</v>
+        <v>63604</v>
       </c>
       <c r="I35" s="34">
-        <v>0.1986551706738601</v>
+        <v>0.19865517067371108</v>
       </c>
       <c r="K35" s="43" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
fineal EUR review, with unified synth quote workbook
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -1840,6 +1840,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1865,7 +1866,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2179,8 +2179,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2206,19 +2206,19 @@
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="179" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="180"/>
-      <c r="K2" s="178" t="s">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="181"/>
+      <c r="K2" s="179" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="181"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="182"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="62"/>
@@ -2357,12 +2357,12 @@
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="58"/>
-      <c r="K9" s="178" t="s">
+      <c r="K9" s="179" t="s">
         <v>155</v>
       </c>
-      <c r="L9" s="179"/>
-      <c r="M9" s="179"/>
-      <c r="N9" s="181"/>
+      <c r="L9" s="180"/>
+      <c r="M9" s="180"/>
+      <c r="N9" s="182"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="62"/>
@@ -2384,7 +2384,9 @@
       <c r="C11" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="87"/>
+      <c r="D11" s="87">
+        <v>41718.524606481478</v>
+      </c>
       <c r="E11" s="59"/>
       <c r="F11" s="58"/>
       <c r="K11" s="120"/>
@@ -2437,8 +2439,8 @@
         <v>94</v>
       </c>
       <c r="D14" s="84" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC1M#0002</v>
+        <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
+        <v>_EURYC1M#0014</v>
       </c>
       <c r="E14" s="59"/>
       <c r="F14" s="58"/>
@@ -2555,14 +2557,8 @@
       <c r="C22" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="74">
-        <f>_xll.qlQuoteValue(D20,Trigger)</f>
-        <v>1</v>
-      </c>
-      <c r="E22" s="73">
-        <f>_xll.qlQuoteValue(E20,Trigger)</f>
-        <v>1</v>
-      </c>
+      <c r="D22" s="74"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="58"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
@@ -2610,7 +2606,7 @@
       <c r="B27" s="62"/>
       <c r="C27" s="66">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="D27" s="65">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2623,11 +2619,11 @@
       <c r="B28" s="62"/>
       <c r="C28" s="64">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>63619</v>
+        <v>63639</v>
       </c>
       <c r="D28" s="63">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.22347000001388923</v>
+        <v>0.2099941941173552</v>
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="58"/>
@@ -2725,11 +2721,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="183" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="183"/>
-      <c r="D1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="185"/>
       <c r="E1" s="31" t="s">
         <v>70</v>
       </c>
@@ -2763,11 +2759,11 @@
       </c>
       <c r="E2" s="14" t="str">
         <f>'1M_Deposits'!K3</f>
-        <v>EUR_YC1MRH_SND#0009</v>
+        <v>EUR_YC1MRH_SND#0000</v>
       </c>
       <c r="F2" s="13">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.2910000000000001E-3</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="12" t="b">
@@ -2781,11 +2777,11 @@
       </c>
       <c r="K2" s="11">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L2" s="10">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41705</v>
+        <v>41723</v>
       </c>
       <c r="M2" s="1">
         <v>30</v>
@@ -2802,11 +2798,11 @@
       </c>
       <c r="E3" s="14" t="str">
         <f>'1M_Deposits'!K4</f>
-        <v>EUR_YC1MRH_SWD#0008</v>
+        <v>EUR_YC1MRH_SWD#0000</v>
       </c>
       <c r="F3" s="13">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.336E-3</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="12" t="b">
@@ -2820,11 +2816,11 @@
       </c>
       <c r="K3" s="11">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L3" s="10">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41711</v>
+        <v>41729</v>
       </c>
       <c r="M3" s="1">
         <v>40</v>
@@ -2841,11 +2837,11 @@
       </c>
       <c r="E4" s="14" t="str">
         <f>'1M_Deposits'!K5</f>
-        <v>EUR_YC1MRH_2WD#0008</v>
+        <v>EUR_YC1MRH_2WD#0000</v>
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3310000000000002E-3</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="12" t="b">
@@ -2859,11 +2855,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41718</v>
+        <v>41736</v>
       </c>
       <c r="M4" s="1">
         <v>50</v>
@@ -2880,11 +2876,11 @@
       </c>
       <c r="E5" s="14" t="str">
         <f>'1M_Deposits'!K6</f>
-        <v>EUR_YC1MRH_3WD#0001</v>
+        <v>EUR_YC1MRH_3WD#0000</v>
       </c>
       <c r="F5" s="13">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3249999999999998E-3</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="12" t="b">
@@ -2898,11 +2894,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41725</v>
+        <v>41743</v>
       </c>
       <c r="M5" s="1">
         <v>60</v>
@@ -2919,11 +2915,11 @@
       </c>
       <c r="E6" s="14" t="str">
         <f>'1M_Deposits'!K7</f>
-        <v>EUR_YC1MRH_1MD#0011</v>
+        <v>EUR_YC1MRH_1MD#0000</v>
       </c>
       <c r="F6" s="13">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3869999999999998E-3</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="12" t="b">
@@ -2937,11 +2933,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41736</v>
+        <v>41753</v>
       </c>
       <c r="M6" s="1">
         <v>70</v>
@@ -3955,11 +3951,11 @@
       </c>
       <c r="D34" s="14" t="str">
         <f t="array" ref="D34:D75">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A34:$A75)</f>
-        <v>H4</v>
+        <v>J4</v>
       </c>
       <c r="E34" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH4</v>
+        <v>EUR_YC1MRH_FUT1MJ4</v>
       </c>
       <c r="F34" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E34,Trigger)</f>
@@ -3997,11 +3993,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D35" s="14" t="str">
-        <v>J4</v>
+        <v>K4</v>
       </c>
       <c r="E35" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MJ4</v>
+        <v>EUR_YC1MRH_FUT1MK4</v>
       </c>
       <c r="F35" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
@@ -4039,11 +4035,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D36" s="14" t="str">
-        <v>K4</v>
+        <v>M4</v>
       </c>
       <c r="E36" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MK4</v>
+        <v>EUR_YC1MRH_FUT1MM4</v>
       </c>
       <c r="F36" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -4081,11 +4077,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D37" s="14" t="str">
-        <v>M4</v>
+        <v>N4</v>
       </c>
       <c r="E37" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM4</v>
+        <v>EUR_YC1MRH_FUT1MN4</v>
       </c>
       <c r="F37" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4123,11 +4119,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D38" s="14" t="str">
-        <v>N4</v>
+        <v>Q4</v>
       </c>
       <c r="E38" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MN4</v>
+        <v>EUR_YC1MRH_FUT1MQ4</v>
       </c>
       <c r="F38" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4165,11 +4161,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D39" s="14" t="str">
-        <v>Q4</v>
+        <v>U4</v>
       </c>
       <c r="E39" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MQ4</v>
+        <v>EUR_YC1MRH_FUT1MU4</v>
       </c>
       <c r="F39" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4207,11 +4203,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D40" s="14" t="str">
-        <v>U4</v>
+        <v>V4</v>
       </c>
       <c r="E40" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU4</v>
+        <v>EUR_YC1MRH_FUT1MV4</v>
       </c>
       <c r="F40" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4249,11 +4245,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D41" s="14" t="str">
-        <v>V4</v>
+        <v>X4</v>
       </c>
       <c r="E41" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MV4</v>
+        <v>EUR_YC1MRH_FUT1MX4</v>
       </c>
       <c r="F41" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4291,11 +4287,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D42" s="14" t="str">
-        <v>X4</v>
+        <v>Z4</v>
       </c>
       <c r="E42" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MX4</v>
+        <v>EUR_YC1MRH_FUT1MZ4</v>
       </c>
       <c r="F42" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4333,11 +4329,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D43" s="14" t="str">
-        <v>Z4</v>
+        <v>F5</v>
       </c>
       <c r="E43" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ4</v>
+        <v>EUR_YC1MRH_FUT1MF5</v>
       </c>
       <c r="F43" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4375,11 +4371,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D44" s="14" t="str">
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E44" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MF5</v>
+        <v>EUR_YC1MRH_FUT1MG5</v>
       </c>
       <c r="F44" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4417,11 +4413,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D45" s="14" t="str">
-        <v>G5</v>
+        <v>H5</v>
       </c>
       <c r="E45" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MG5</v>
+        <v>EUR_YC1MRH_FUT1MH5</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4459,11 +4455,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D46" s="14" t="str">
-        <v>H5</v>
+        <v>M5</v>
       </c>
       <c r="E46" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH5</v>
+        <v>EUR_YC1MRH_FUT1MM5</v>
       </c>
       <c r="F46" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4501,11 +4497,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D47" s="14" t="str">
-        <v>M5</v>
+        <v>U5</v>
       </c>
       <c r="E47" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM5</v>
+        <v>EUR_YC1MRH_FUT1MU5</v>
       </c>
       <c r="F47" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4543,11 +4539,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D48" s="14" t="str">
-        <v>U5</v>
+        <v>Z5</v>
       </c>
       <c r="E48" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU5</v>
+        <v>EUR_YC1MRH_FUT1MZ5</v>
       </c>
       <c r="F48" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
@@ -4585,11 +4581,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D49" s="14" t="str">
-        <v>Z5</v>
+        <v>H6</v>
       </c>
       <c r="E49" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ5</v>
+        <v>EUR_YC1MRH_FUT1MH6</v>
       </c>
       <c r="F49" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
@@ -4627,11 +4623,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D50" s="14" t="str">
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="E50" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH6</v>
+        <v>EUR_YC1MRH_FUT1MM6</v>
       </c>
       <c r="F50" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
@@ -4669,11 +4665,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D51" s="14" t="str">
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="E51" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM6</v>
+        <v>EUR_YC1MRH_FUT1MU6</v>
       </c>
       <c r="F51" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
@@ -4711,11 +4707,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D52" s="14" t="str">
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="E52" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU6</v>
+        <v>EUR_YC1MRH_FUT1MZ6</v>
       </c>
       <c r="F52" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
@@ -4753,11 +4749,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D53" s="14" t="str">
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="E53" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ6</v>
+        <v>EUR_YC1MRH_FUT1MH7</v>
       </c>
       <c r="F53" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
@@ -4795,11 +4791,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D54" s="14" t="str">
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="E54" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH7</v>
+        <v>EUR_YC1MRH_FUT1MM7</v>
       </c>
       <c r="F54" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
@@ -4837,11 +4833,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D55" s="14" t="str">
-        <v>M7</v>
+        <v>U7</v>
       </c>
       <c r="E55" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM7</v>
+        <v>EUR_YC1MRH_FUT1MU7</v>
       </c>
       <c r="F55" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
@@ -4879,11 +4875,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D56" s="14" t="str">
-        <v>U7</v>
+        <v>Z7</v>
       </c>
       <c r="E56" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU7</v>
+        <v>EUR_YC1MRH_FUT1MZ7</v>
       </c>
       <c r="F56" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
@@ -4921,11 +4917,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D57" s="14" t="str">
-        <v>Z7</v>
+        <v>H8</v>
       </c>
       <c r="E57" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ7</v>
+        <v>EUR_YC1MRH_FUT1MH8</v>
       </c>
       <c r="F57" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
@@ -4963,11 +4959,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D58" s="14" t="str">
-        <v>H8</v>
+        <v>M8</v>
       </c>
       <c r="E58" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH8</v>
+        <v>EUR_YC1MRH_FUT1MM8</v>
       </c>
       <c r="F58" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
@@ -5005,11 +5001,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D59" s="14" t="str">
-        <v>M8</v>
+        <v>U8</v>
       </c>
       <c r="E59" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM8</v>
+        <v>EUR_YC1MRH_FUT1MU8</v>
       </c>
       <c r="F59" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
@@ -5047,11 +5043,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D60" s="14" t="str">
-        <v>U8</v>
+        <v>Z8</v>
       </c>
       <c r="E60" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU8</v>
+        <v>EUR_YC1MRH_FUT1MZ8</v>
       </c>
       <c r="F60" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
@@ -5089,11 +5085,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D61" s="14" t="str">
-        <v>Z8</v>
+        <v>H9</v>
       </c>
       <c r="E61" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ8</v>
+        <v>EUR_YC1MRH_FUT1MH9</v>
       </c>
       <c r="F61" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
@@ -5131,11 +5127,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D62" s="14" t="str">
-        <v>H9</v>
+        <v>M9</v>
       </c>
       <c r="E62" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH9</v>
+        <v>EUR_YC1MRH_FUT1MM9</v>
       </c>
       <c r="F62" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
@@ -5173,11 +5169,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D63" s="14" t="str">
-        <v>M9</v>
+        <v>U9</v>
       </c>
       <c r="E63" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM9</v>
+        <v>EUR_YC1MRH_FUT1MU9</v>
       </c>
       <c r="F63" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
@@ -5215,11 +5211,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D64" s="14" t="str">
-        <v>U9</v>
+        <v>Z9</v>
       </c>
       <c r="E64" s="14" t="str">
         <f t="shared" ref="E64:E95" si="4">RateHelperPrefix&amp;"_"&amp;$B64&amp;$C64&amp;$D64</f>
-        <v>EUR_YC1MRH_FUT1MU9</v>
+        <v>EUR_YC1MRH_FUT1MZ9</v>
       </c>
       <c r="F64" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
@@ -5257,11 +5253,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D65" s="14" t="str">
-        <v>Z9</v>
+        <v>H0</v>
       </c>
       <c r="E65" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MZ9</v>
+        <v>EUR_YC1MRH_FUT1MH0</v>
       </c>
       <c r="F65" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
@@ -5299,11 +5295,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D66" s="14" t="str">
-        <v>H0</v>
+        <v>M0</v>
       </c>
       <c r="E66" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MH0</v>
+        <v>EUR_YC1MRH_FUT1MM0</v>
       </c>
       <c r="F66" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
@@ -5341,11 +5337,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D67" s="14" t="str">
-        <v>M0</v>
+        <v>U0</v>
       </c>
       <c r="E67" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MM0</v>
+        <v>EUR_YC1MRH_FUT1MU0</v>
       </c>
       <c r="F67" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
@@ -5383,11 +5379,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D68" s="14" t="str">
-        <v>U0</v>
+        <v>Z0</v>
       </c>
       <c r="E68" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MU0</v>
+        <v>EUR_YC1MRH_FUT1MZ0</v>
       </c>
       <c r="F68" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
@@ -5425,11 +5421,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D69" s="14" t="str">
-        <v>Z0</v>
+        <v>H1</v>
       </c>
       <c r="E69" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MZ0</v>
+        <v>EUR_YC1MRH_FUT1MH1</v>
       </c>
       <c r="F69" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
@@ -5467,11 +5463,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D70" s="14" t="str">
-        <v>H1</v>
+        <v>M1</v>
       </c>
       <c r="E70" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MH1</v>
+        <v>EUR_YC1MRH_FUT1MM1</v>
       </c>
       <c r="F70" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
@@ -5509,11 +5505,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D71" s="14" t="str">
-        <v>M1</v>
+        <v>U1</v>
       </c>
       <c r="E71" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MM1</v>
+        <v>EUR_YC1MRH_FUT1MU1</v>
       </c>
       <c r="F71" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
@@ -5551,11 +5547,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D72" s="14" t="str">
-        <v>U1</v>
+        <v>Z1</v>
       </c>
       <c r="E72" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MU1</v>
+        <v>EUR_YC1MRH_FUT1MZ1</v>
       </c>
       <c r="F72" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
@@ -5593,11 +5589,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D73" s="14" t="str">
-        <v>Z1</v>
+        <v>H2</v>
       </c>
       <c r="E73" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MZ1</v>
+        <v>EUR_YC1MRH_FUT1MH2</v>
       </c>
       <c r="F73" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
@@ -5635,11 +5631,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D74" s="14" t="str">
-        <v>H2</v>
+        <v>M2</v>
       </c>
       <c r="E74" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MH2</v>
+        <v>EUR_YC1MRH_FUT1MM2</v>
       </c>
       <c r="F74" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
@@ -5677,11 +5673,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D75" s="7" t="str">
-        <v>M2</v>
+        <v>U2</v>
       </c>
       <c r="E75" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>EUR_YC1MRH_FUT1MM2</v>
+        <v>EUR_YC1MRH_FUT1MU2</v>
       </c>
       <c r="F75" s="27" t="e">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
@@ -5720,11 +5716,11 @@
       </c>
       <c r="E76" s="21" t="str">
         <f>'1M_Swaps'!L6</f>
-        <v>EUR_YC1MRH_2X1S#0001</v>
+        <v>EUR_YC1MRH_2X1S#0000</v>
       </c>
       <c r="F76" s="20">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>2.0800000000000003E-3</v>
+        <v>2.3899999999999998E-3</v>
       </c>
       <c r="G76" s="20">
         <f>_xll.qlSwapRateHelperSpread($E76,Trigger)</f>
@@ -5741,11 +5737,11 @@
       </c>
       <c r="K76" s="18">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L76" s="17">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>41765</v>
+        <v>41785</v>
       </c>
       <c r="M76" s="22"/>
     </row>
@@ -5759,11 +5755,11 @@
       </c>
       <c r="E77" s="14" t="str">
         <f>'1M_Swaps'!L7</f>
-        <v>EUR_YC1MRH_3X1S#0001</v>
+        <v>EUR_YC1MRH_3X1S#0000</v>
       </c>
       <c r="F77" s="13">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
-        <v>1.98E-3</v>
+        <v>2.3799999999999997E-3</v>
       </c>
       <c r="G77" s="13">
         <f>_xll.qlSwapRateHelperSpread($E77,Trigger)</f>
@@ -5780,11 +5776,11 @@
       </c>
       <c r="K77" s="11">
         <f>_xll.qlRateHelperEarliestDate($E77,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L77" s="10">
         <f>_xll.qlRateHelperLatestDate($E77,Trigger)</f>
-        <v>41796</v>
+        <v>41814</v>
       </c>
       <c r="M77" s="25"/>
     </row>
@@ -5798,11 +5794,11 @@
       </c>
       <c r="E78" s="14" t="str">
         <f>'1M_Swaps'!L8</f>
-        <v>EUR_YC1MRH_4X1S#0001</v>
+        <v>EUR_YC1MRH_4X1S#0000</v>
       </c>
       <c r="F78" s="13">
         <f>_xll.qlRateHelperQuoteValue($E78,Trigger)</f>
-        <v>1.9E-3</v>
+        <v>2.3699999999999997E-3</v>
       </c>
       <c r="G78" s="13">
         <f>_xll.qlSwapRateHelperSpread($E78,Trigger)</f>
@@ -5819,11 +5815,11 @@
       </c>
       <c r="K78" s="11">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L78" s="10">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>41827</v>
+        <v>41844</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -5836,11 +5832,11 @@
       </c>
       <c r="E79" s="14" t="str">
         <f>'1M_Swaps'!L9</f>
-        <v>EUR_YC1MRH_5X1S#0001</v>
+        <v>EUR_YC1MRH_5X1S#0000</v>
       </c>
       <c r="F79" s="13">
         <f>_xll.qlRateHelperQuoteValue($E79,Trigger)</f>
-        <v>1.8400000000000001E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G79" s="13">
         <f>_xll.qlSwapRateHelperSpread($E79,Trigger)</f>
@@ -5857,11 +5853,11 @@
       </c>
       <c r="K79" s="11">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L79" s="10">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>41857</v>
+        <v>41876</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5874,11 +5870,11 @@
       </c>
       <c r="E80" s="14" t="str">
         <f>'1M_Swaps'!L10</f>
-        <v>EUR_YC1MRH_6X1S#0001</v>
+        <v>EUR_YC1MRH_6X1S#0000</v>
       </c>
       <c r="F80" s="13">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
-        <v>1.7899999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G80" s="13">
         <f>_xll.qlSwapRateHelperSpread($E80,Trigger)</f>
@@ -5895,11 +5891,11 @@
       </c>
       <c r="K80" s="11">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L80" s="10">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>41890</v>
+        <v>41906</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
@@ -5912,11 +5908,11 @@
       </c>
       <c r="E81" s="14" t="str">
         <f>'1M_Swaps'!L11</f>
-        <v>EUR_YC1MRH_7X1S#0001</v>
+        <v>EUR_YC1MRH_7X1S#0000</v>
       </c>
       <c r="F81" s="13">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
-        <v>1.7699999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G81" s="13">
         <f>_xll.qlSwapRateHelperSpread($E81,Trigger)</f>
@@ -5933,11 +5929,11 @@
       </c>
       <c r="K81" s="11">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L81" s="10">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>41918</v>
+        <v>41936</v>
       </c>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.2">
@@ -5950,11 +5946,11 @@
       </c>
       <c r="E82" s="14" t="str">
         <f>'1M_Swaps'!L12</f>
-        <v>EUR_YC1MRH_8X1S#0001</v>
+        <v>EUR_YC1MRH_8X1S#0000</v>
       </c>
       <c r="F82" s="13">
         <f>_xll.qlRateHelperQuoteValue($E82,Trigger)</f>
-        <v>1.7599999999999998E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G82" s="13">
         <f>_xll.qlSwapRateHelperSpread($E82,Trigger)</f>
@@ -5971,11 +5967,11 @@
       </c>
       <c r="K82" s="11">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L82" s="10">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>41949</v>
+        <v>41967</v>
       </c>
     </row>
     <row r="83" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5988,11 +5984,11 @@
       </c>
       <c r="E83" s="14" t="str">
         <f>'1M_Swaps'!L13</f>
-        <v>EUR_YC1MRH_9X1S#0001</v>
+        <v>EUR_YC1MRH_9X1S#0000</v>
       </c>
       <c r="F83" s="13">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
-        <v>1.7499999999999998E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G83" s="13">
         <f>_xll.qlSwapRateHelperSpread($E83,Trigger)</f>
@@ -6009,11 +6005,11 @@
       </c>
       <c r="K83" s="11">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L83" s="10">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>41981</v>
+        <v>41997</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
@@ -6026,11 +6022,11 @@
       </c>
       <c r="E84" s="14" t="str">
         <f>'1M_Swaps'!L14</f>
-        <v>EUR_YC1MRH_10X1S#0001</v>
+        <v>EUR_YC1MRH_10X1S#0000</v>
       </c>
       <c r="F84" s="13">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
-        <v>1.7399999999999998E-3</v>
+        <v>2.3400000000000001E-3</v>
       </c>
       <c r="G84" s="13">
         <f>_xll.qlSwapRateHelperSpread($E84,Trigger)</f>
@@ -6047,11 +6043,11 @@
       </c>
       <c r="K84" s="11">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L84" s="10">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>42010</v>
+        <v>42030</v>
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.2">
@@ -6064,11 +6060,11 @@
       </c>
       <c r="E85" s="14" t="str">
         <f>'1M_Swaps'!L15</f>
-        <v>EUR_YC1MRH_11X1S#0001</v>
+        <v>EUR_YC1MRH_11X1S#0000</v>
       </c>
       <c r="F85" s="13">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
-        <v>1.72E-3</v>
+        <v>2.3499999999999997E-3</v>
       </c>
       <c r="G85" s="13">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
@@ -6085,11 +6081,11 @@
       </c>
       <c r="K85" s="11">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L85" s="10">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>42041</v>
+        <v>42059</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
@@ -6102,11 +6098,11 @@
       </c>
       <c r="E86" s="7" t="str">
         <f>'1M_Swaps'!L16</f>
-        <v>EUR_YC1MRH_12X1S#0001</v>
+        <v>EUR_YC1MRH_12X1S#0000</v>
       </c>
       <c r="F86" s="6">
         <f>_xll.qlRateHelperQuoteValue($E86,Trigger)</f>
-        <v>1.7099999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="G86" s="6">
         <f>_xll.qlSwapRateHelperSpread($E86,Trigger)</f>
@@ -6123,11 +6119,11 @@
       </c>
       <c r="K86" s="4">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L86" s="3">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>42069</v>
+        <v>42087</v>
       </c>
     </row>
     <row r="87" spans="2:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8112,11 +8108,11 @@
       </c>
       <c r="E131" s="21" t="str">
         <f>'1M_SwapsFromBasis'!L6</f>
-        <v>EUR_YC1MRH_AB1EBASIS1Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS1Y#0000</v>
       </c>
       <c r="F131" s="20">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
-        <v>1.7400000000000002E-3</v>
+        <v>2.3900000000000002E-3</v>
       </c>
       <c r="G131" s="20">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
@@ -8133,11 +8129,11 @@
       </c>
       <c r="K131" s="18">
         <f>_xll.qlRateHelperEarliestDate($E131,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L131" s="17">
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
-        <v>42069</v>
+        <v>42087</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
@@ -8154,11 +8150,11 @@
       </c>
       <c r="E132" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L7</f>
-        <v>EUR_YC1MRH_AB1EBASIS15M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15M#0000</v>
       </c>
       <c r="F132" s="13">
         <f>_xll.qlRateHelperQuoteValue($E132,Trigger)</f>
-        <v>1.519E-3</v>
+        <v>2.2680000000000001E-3</v>
       </c>
       <c r="G132" s="13">
         <f>_xll.qlSwapRateHelperSpread($E132,Trigger)</f>
@@ -8175,11 +8171,11 @@
       </c>
       <c r="K132" s="11">
         <f>_xll.qlRateHelperEarliestDate($E132,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L132" s="10">
         <f>_xll.qlRateHelperLatestDate($E132,Trigger)</f>
-        <v>42163</v>
+        <v>42179</v>
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.2">
@@ -8196,11 +8192,11 @@
       </c>
       <c r="E133" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L8</f>
-        <v>EUR_YC1MRH_AB1EBASIS18M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18M#0000</v>
       </c>
       <c r="F133" s="13">
         <f>_xll.qlRateHelperQuoteValue($E133,Trigger)</f>
-        <v>1.8579999999999998E-3</v>
+        <v>2.5270000000000002E-3</v>
       </c>
       <c r="G133" s="13">
         <f>_xll.qlSwapRateHelperSpread($E133,Trigger)</f>
@@ -8217,11 +8213,11 @@
       </c>
       <c r="K133" s="11">
         <f>_xll.qlRateHelperEarliestDate($E133,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L133" s="10">
         <f>_xll.qlRateHelperLatestDate($E133,Trigger)</f>
-        <v>42254</v>
+        <v>42271</v>
       </c>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.2">
@@ -8238,11 +8234,11 @@
       </c>
       <c r="E134" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L9</f>
-        <v>EUR_YC1MRH_AB1EBASIS21M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21M#0000</v>
       </c>
       <c r="F134" s="13">
         <f>_xll.qlRateHelperQuoteValue($E134,Trigger)</f>
-        <v>1.7780000000000005E-3</v>
+        <v>2.5069999999999992E-3</v>
       </c>
       <c r="G134" s="13">
         <f>_xll.qlSwapRateHelperSpread($E134,Trigger)</f>
@@ -8259,11 +8255,11 @@
       </c>
       <c r="K134" s="11">
         <f>_xll.qlRateHelperEarliestDate($E134,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L134" s="10">
         <f>_xll.qlRateHelperLatestDate($E134,Trigger)</f>
-        <v>42345</v>
+        <v>42362</v>
       </c>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.2">
@@ -8280,11 +8276,11 @@
       </c>
       <c r="E135" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L10</f>
-        <v>EUR_YC1MRH_AB1EBASIS2Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS2Y#0000</v>
       </c>
       <c r="F135" s="13">
         <f>_xll.qlRateHelperQuoteValue($E135,Trigger)</f>
-        <v>2.1199999999999991E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="G135" s="13">
         <f>_xll.qlSwapRateHelperSpread($E135,Trigger)</f>
@@ -8301,11 +8297,11 @@
       </c>
       <c r="K135" s="11">
         <f>_xll.qlRateHelperEarliestDate($E135,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L135" s="10">
         <f>_xll.qlRateHelperLatestDate($E135,Trigger)</f>
-        <v>42436</v>
+        <v>42453</v>
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.2">
@@ -8322,11 +8318,11 @@
       </c>
       <c r="E136" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L11</f>
-        <v>EUR_YC1MRH_AB1EBASIS3Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS3Y#0000</v>
       </c>
       <c r="F136" s="13">
         <f>_xll.qlRateHelperQuoteValue($E136,Trigger)</f>
-        <v>3.3199999999999996E-3</v>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="G136" s="13">
         <f>_xll.qlSwapRateHelperSpread($E136,Trigger)</f>
@@ -8343,11 +8339,11 @@
       </c>
       <c r="K136" s="11">
         <f>_xll.qlRateHelperEarliestDate($E136,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L136" s="10">
         <f>_xll.qlRateHelperLatestDate($E136,Trigger)</f>
-        <v>42800</v>
+        <v>42818</v>
       </c>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.2">
@@ -8364,11 +8360,11 @@
       </c>
       <c r="E137" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L12</f>
-        <v>EUR_YC1MRH_AB1EBASIS4Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS4Y#0000</v>
       </c>
       <c r="F137" s="13">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>5.0799999999999994E-3</v>
+        <v>5.6599999999999992E-3</v>
       </c>
       <c r="G137" s="13">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -8385,11 +8381,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>43165</v>
+        <v>43185</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8406,11 +8402,11 @@
       </c>
       <c r="E138" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L13</f>
-        <v>EUR_YC1MRH_AB1EBASIS5Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS5Y#0000</v>
       </c>
       <c r="F138" s="13">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>6.9899999999999988E-3</v>
+        <v>7.5299999999999994E-3</v>
       </c>
       <c r="G138" s="13">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -8427,11 +8423,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>43530</v>
+        <v>43549</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8448,11 +8444,11 @@
       </c>
       <c r="E139" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L14</f>
-        <v>EUR_YC1MRH_AB1EBASIS6Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS6Y#0000</v>
       </c>
       <c r="F139" s="13">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>8.9500000000000014E-3</v>
+        <v>9.4400000000000005E-3</v>
       </c>
       <c r="G139" s="13">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -8469,11 +8465,11 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>43896</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
@@ -8490,11 +8486,11 @@
       </c>
       <c r="E140" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L15</f>
-        <v>EUR_YC1MRH_AB1EBASIS7Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS7Y#0000</v>
       </c>
       <c r="F140" s="13">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>1.0840000000000001E-2</v>
+        <v>1.1300000000000001E-2</v>
       </c>
       <c r="G140" s="13">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -8511,11 +8507,11 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>44263</v>
+        <v>44279</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
@@ -8532,11 +8528,11 @@
       </c>
       <c r="E141" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L16</f>
-        <v>EUR_YC1MRH_AB1EBASIS8Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS8Y#0000</v>
       </c>
       <c r="F141" s="13">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>1.26E-2</v>
+        <v>1.3059999999999999E-2</v>
       </c>
       <c r="G141" s="13">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -8553,11 +8549,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>44627</v>
+        <v>44644</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8574,11 +8570,11 @@
       </c>
       <c r="E142" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L17</f>
-        <v>EUR_YC1MRH_AB1EBASIS9Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS9Y#0000</v>
       </c>
       <c r="F142" s="13">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>1.4199999999999999E-2</v>
+        <v>1.4659999999999999E-2</v>
       </c>
       <c r="G142" s="13">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -8595,11 +8591,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>44991</v>
+        <v>45009</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8616,11 +8612,11 @@
       </c>
       <c r="E143" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L18</f>
-        <v>EUR_YC1MRH_AB1EBASIS10Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS10Y#0000</v>
       </c>
       <c r="F143" s="13">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>1.566E-2</v>
+        <v>1.6119999999999999E-2</v>
       </c>
       <c r="G143" s="13">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -8637,11 +8633,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>45357</v>
+        <v>45376</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8658,11 +8654,11 @@
       </c>
       <c r="E144" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L19</f>
-        <v>EUR_YC1MRH_AB1EBASIS11Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS11Y#0000</v>
       </c>
       <c r="F144" s="13">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>1.694E-2</v>
+        <v>1.7409999999999998E-2</v>
       </c>
       <c r="G144" s="13">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -8679,11 +8675,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>45722</v>
+        <v>45740</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8700,11 +8696,11 @@
       </c>
       <c r="E145" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L20</f>
-        <v>EUR_YC1MRH_AB1EBASIS12Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS12Y#0000</v>
       </c>
       <c r="F145" s="13">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>1.8030000000000001E-2</v>
+        <v>1.8530000000000001E-2</v>
       </c>
       <c r="G145" s="13">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -8721,11 +8717,11 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>46087</v>
+        <v>46105</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
@@ -8742,11 +8738,11 @@
       </c>
       <c r="E146" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L21</f>
-        <v>EUR_YC1MRH_AB1EBASIS13Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS13Y#0000</v>
       </c>
       <c r="F146" s="13">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>1.8994999999999998E-2</v>
+        <v>1.95E-2</v>
       </c>
       <c r="G146" s="13">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -8763,11 +8759,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>46454</v>
+        <v>46470</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8784,11 +8780,11 @@
       </c>
       <c r="E147" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L22</f>
-        <v>EUR_YC1MRH_AB1EBASIS14Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS14Y#0000</v>
       </c>
       <c r="F147" s="13">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>1.9824000000000001E-2</v>
+        <v>2.0336999999999997E-2</v>
       </c>
       <c r="G147" s="13">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -8805,11 +8801,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46818</v>
+        <v>46836</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8826,11 +8822,11 @@
       </c>
       <c r="E148" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L23</f>
-        <v>EUR_YC1MRH_AB1EBASIS15Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15Y#0000</v>
       </c>
       <c r="F148" s="13">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>2.051E-2</v>
+        <v>2.1029999999999997E-2</v>
       </c>
       <c r="G148" s="13">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -8847,11 +8843,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>47183</v>
+        <v>47203</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8868,11 +8864,11 @@
       </c>
       <c r="E149" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L24</f>
-        <v>EUR_YC1MRH_AB1EBASIS16Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS16Y#0000</v>
       </c>
       <c r="F149" s="13">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>2.1069000000000001E-2</v>
+        <v>2.1596000000000001E-2</v>
       </c>
       <c r="G149" s="13">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -8889,11 +8885,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>47548</v>
+        <v>47567</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8910,11 +8906,11 @@
       </c>
       <c r="E150" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L25</f>
-        <v>EUR_YC1MRH_AB1EBASIS17Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS17Y#0000</v>
       </c>
       <c r="F150" s="13">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>2.1519999999999997E-2</v>
+        <v>2.2054999999999998E-2</v>
       </c>
       <c r="G150" s="13">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -8931,11 +8927,11 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>47913</v>
+        <v>47931</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
@@ -8952,11 +8948,11 @@
       </c>
       <c r="E151" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L26</f>
-        <v>EUR_YC1MRH_AB1EBASIS18Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18Y#0000</v>
       </c>
       <c r="F151" s="13">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>2.1885000000000002E-2</v>
+        <v>2.2428E-2</v>
       </c>
       <c r="G151" s="13">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -8973,11 +8969,11 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>48281</v>
+        <v>48297</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
@@ -8994,11 +8990,11 @@
       </c>
       <c r="E152" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L27</f>
-        <v>EUR_YC1MRH_AB1EBASIS19Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS19Y#0000</v>
       </c>
       <c r="F152" s="13">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>2.2164999999999997E-2</v>
+        <v>2.2726E-2</v>
       </c>
       <c r="G152" s="13">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -9015,11 +9011,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>48645</v>
+        <v>48662</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -9036,11 +9032,11 @@
       </c>
       <c r="E153" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L28</f>
-        <v>EUR_YC1MRH_AB1EBASIS20Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS20Y#0000</v>
       </c>
       <c r="F153" s="13">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>2.2390000000000004E-2</v>
+        <v>2.2969999999999997E-2</v>
       </c>
       <c r="G153" s="13">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -9057,11 +9053,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>49009</v>
+        <v>49027</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -9078,11 +9074,11 @@
       </c>
       <c r="E154" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L29</f>
-        <v>EUR_YC1MRH_AB1EBASIS21Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21Y#0000</v>
       </c>
       <c r="F154" s="13">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>2.2582000000000001E-2</v>
+        <v>2.3169999999999996E-2</v>
       </c>
       <c r="G154" s="13">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -9099,11 +9095,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>49374</v>
+        <v>49395</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9120,11 +9116,11 @@
       </c>
       <c r="E155" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L30</f>
-        <v>EUR_YC1MRH_AB1EBASIS22Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS22Y#0000</v>
       </c>
       <c r="F155" s="13">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>2.2750999999999997E-2</v>
+        <v>2.3348000000000004E-2</v>
       </c>
       <c r="G155" s="13">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -9141,11 +9137,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>49740</v>
+        <v>49758</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9162,11 +9158,11 @@
       </c>
       <c r="E156" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L31</f>
-        <v>EUR_YC1MRH_AB1EBASIS23Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS23Y#0000</v>
       </c>
       <c r="F156" s="13">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>2.2876999999999998E-2</v>
+        <v>2.3482000000000003E-2</v>
       </c>
       <c r="G156" s="13">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -9183,11 +9179,11 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>50105</v>
+        <v>50123</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
@@ -9204,11 +9200,11 @@
       </c>
       <c r="E157" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L32</f>
-        <v>EUR_YC1MRH_AB1EBASIS24Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS24Y#0000</v>
       </c>
       <c r="F157" s="13">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>2.299E-2</v>
+        <v>2.3591999999999998E-2</v>
       </c>
       <c r="G157" s="13">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -9225,11 +9221,11 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>50472</v>
+        <v>50488</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
@@ -9246,11 +9242,11 @@
       </c>
       <c r="E158" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L33</f>
-        <v>EUR_YC1MRH_AB1EBASIS25Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS25Y#0000</v>
       </c>
       <c r="F158" s="13">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>2.307E-2</v>
+        <v>2.368E-2</v>
       </c>
       <c r="G158" s="13">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -9267,11 +9263,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50836</v>
+        <v>50853</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9288,11 +9284,11 @@
       </c>
       <c r="E159" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L34</f>
-        <v>EUR_YC1MRH_AB1EBASIS26Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS26Y#0000</v>
       </c>
       <c r="F159" s="13">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>2.3137000000000005E-2</v>
+        <v>2.3744999999999999E-2</v>
       </c>
       <c r="G159" s="13">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -9309,11 +9305,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>51201</v>
+        <v>51221</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9330,11 +9326,11 @@
       </c>
       <c r="E160" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L35</f>
-        <v>EUR_YC1MRH_AB1EBASIS27Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS27Y#0000</v>
       </c>
       <c r="F160" s="13">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>2.3181E-2</v>
+        <v>2.3795999999999998E-2</v>
       </c>
       <c r="G160" s="13">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -9351,11 +9347,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>51566</v>
+        <v>51585</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9372,11 +9368,11 @@
       </c>
       <c r="E161" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L36</f>
-        <v>EUR_YC1MRH_AB1EBASIS28Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS28Y#0000</v>
       </c>
       <c r="F161" s="13">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>2.3223000000000001E-2</v>
+        <v>2.3836E-2</v>
       </c>
       <c r="G161" s="13">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -9393,11 +9389,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>51931</v>
+        <v>51949</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9414,11 +9410,11 @@
       </c>
       <c r="E162" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L37</f>
-        <v>EUR_YC1MRH_AB1EBASIS29Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS29Y#0000</v>
       </c>
       <c r="F162" s="13">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>2.3251999999999998E-2</v>
+        <v>2.3864E-2</v>
       </c>
       <c r="G162" s="13">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -9435,11 +9431,11 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>52296</v>
+        <v>52314</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.2">
@@ -9456,11 +9452,11 @@
       </c>
       <c r="E163" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L38</f>
-        <v>EUR_YC1MRH_AB1EBASIS30Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS30Y#0000</v>
       </c>
       <c r="F163" s="13">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>2.3279999999999999E-2</v>
+        <v>2.3899999999999998E-2</v>
       </c>
       <c r="G163" s="13">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -9477,11 +9473,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>52663</v>
+        <v>52680</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9498,11 +9494,11 @@
       </c>
       <c r="E164" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L39</f>
-        <v>EUR_YC1MRH_AB1EBASIS35Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS35Y#0000</v>
       </c>
       <c r="F164" s="13">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>2.3477999999999999E-2</v>
+        <v>2.4135999999999998E-2</v>
       </c>
       <c r="G164" s="13">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
@@ -9519,11 +9515,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>54490</v>
+        <v>54506</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9540,11 +9536,11 @@
       </c>
       <c r="E165" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L40</f>
-        <v>EUR_YC1MRH_AB1EBASIS40Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS40Y#0000</v>
       </c>
       <c r="F165" s="13">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>2.3699999999999999E-2</v>
+        <v>2.4420000000000001E-2</v>
       </c>
       <c r="G165" s="13">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -9561,11 +9557,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>56314</v>
+        <v>56332</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9582,11 +9578,11 @@
       </c>
       <c r="E166" s="14" t="str">
         <f>'1M_SwapsFromBasis'!L41</f>
-        <v>EUR_YC1MRH_AB1EBASIS50Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS50Y#0000</v>
       </c>
       <c r="F166" s="13">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>2.3970000000000002E-2</v>
+        <v>2.4759999999999997E-2</v>
       </c>
       <c r="G166" s="13">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -9603,11 +9599,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>59967</v>
+        <v>59985</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9624,11 +9620,11 @@
       </c>
       <c r="E167" s="7" t="str">
         <f>'1M_SwapsFromBasis'!L42</f>
-        <v>EUR_YC1MRH_AB1EBASIS60Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS60Y#0000</v>
       </c>
       <c r="F167" s="6">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>2.418E-2</v>
+        <v>2.4970000000000003E-2</v>
       </c>
       <c r="G167" s="6">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -9645,11 +9641,11 @@
       </c>
       <c r="K167" s="4">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="L167" s="3">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>63619</v>
+        <v>63639</v>
       </c>
     </row>
   </sheetData>
@@ -9668,7 +9664,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -9689,10 +9685,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="186" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="187"/>
       <c r="D1" s="54" t="s">
         <v>79</v>
       </c>
@@ -9724,7 +9720,7 @@
       </c>
       <c r="E2" s="41">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.2910000000000001E-3</v>
       </c>
       <c r="F2" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -9732,14 +9728,14 @@
       </c>
       <c r="G2" s="40">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H2" s="39">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41705</v>
+        <v>41723</v>
       </c>
       <c r="I2" s="34">
-        <v>0.99999375281680536</v>
+        <v>0.9999939555920907</v>
       </c>
       <c r="K2" s="92" t="s">
         <v>192</v>
@@ -9760,7 +9756,7 @@
       </c>
       <c r="E3" s="41">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.336E-3</v>
       </c>
       <c r="F3" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -9768,14 +9764,14 @@
       </c>
       <c r="G3" s="40">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H3" s="39">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41711</v>
+        <v>41729</v>
       </c>
       <c r="I3" s="34">
-        <v>0.99995627135672238</v>
+        <v>0.99995638801319908</v>
       </c>
       <c r="K3" s="92" t="s">
         <v>112</v>
@@ -9796,7 +9792,7 @@
       </c>
       <c r="E4" s="41">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3310000000000002E-3</v>
       </c>
       <c r="F4" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -9804,14 +9800,14 @@
       </c>
       <c r="G4" s="40">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H4" s="39">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41718</v>
+        <v>41736</v>
       </c>
       <c r="I4" s="34">
-        <v>0.99991254653766592</v>
+        <v>0.99991242989141771</v>
       </c>
       <c r="K4" s="92" t="s">
         <v>113</v>
@@ -9832,7 +9828,7 @@
       </c>
       <c r="E5" s="41">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3249999999999998E-3</v>
       </c>
       <c r="F5" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -9840,14 +9836,14 @@
       </c>
       <c r="G5" s="40">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H5" s="39">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41725</v>
+        <v>41743</v>
       </c>
       <c r="I5" s="34">
-        <v>0.99986882554232903</v>
+        <v>0.99986748422942306</v>
       </c>
       <c r="K5" s="92" t="s">
         <v>114</v>
@@ -9869,7 +9865,7 @@
       </c>
       <c r="E6" s="41">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>2.2490000000000001E-3</v>
+        <v>2.3869999999999998E-3</v>
       </c>
       <c r="F6" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -9877,14 +9873,14 @@
       </c>
       <c r="G6" s="40">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H6" s="39">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41736</v>
+        <v>41753</v>
       </c>
       <c r="I6" s="34">
-        <v>0.99980012884535341</v>
+        <v>0.99979509754911167</v>
       </c>
       <c r="K6" s="92" t="s">
         <v>115</v>
@@ -9896,7 +9892,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_RateHelpersSelected#0002</v>
+        <v>EUR_YC1MRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="44" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -9907,7 +9903,7 @@
       </c>
       <c r="E7" s="41">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>2.0800000000000003E-3</v>
+        <v>2.3899999999999998E-3</v>
       </c>
       <c r="F7" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -9915,14 +9911,14 @@
       </c>
       <c r="G7" s="40">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H7" s="39">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41765</v>
+        <v>41785</v>
       </c>
       <c r="I7" s="34">
-        <v>0.99964153905229658</v>
+        <v>0.9995801647289998</v>
       </c>
       <c r="K7" s="92" t="s">
         <v>116</v>
@@ -9937,7 +9933,7 @@
       </c>
       <c r="E8" s="41">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1.98E-3</v>
+        <v>2.3799999999999997E-3</v>
       </c>
       <c r="F8" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -9945,14 +9941,14 @@
       </c>
       <c r="G8" s="40">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H8" s="39">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41796</v>
+        <v>41814</v>
       </c>
       <c r="I8" s="34">
-        <v>0.99948809465016319</v>
+        <v>0.99938701029549082</v>
       </c>
       <c r="K8" s="92" t="s">
         <v>117</v>
@@ -9967,7 +9963,7 @@
       </c>
       <c r="E9" s="41">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1.9E-3</v>
+        <v>2.3699999999999997E-3</v>
       </c>
       <c r="F9" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -9975,14 +9971,14 @@
       </c>
       <c r="G9" s="40">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H9" s="39">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41827</v>
+        <v>41844</v>
       </c>
       <c r="I9" s="34">
-        <v>0.99934506839470694</v>
+        <v>0.99918388080942111</v>
       </c>
       <c r="K9" s="92" t="s">
         <v>118</v>
@@ -9997,7 +9993,7 @@
       </c>
       <c r="E10" s="41">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>1.8400000000000001E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F10" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -10005,14 +10001,14 @@
       </c>
       <c r="G10" s="40">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41857</v>
+        <v>41876</v>
       </c>
       <c r="I10" s="34">
-        <v>0.99921238906769139</v>
+        <v>0.99897000838075511</v>
       </c>
       <c r="K10" s="92" t="s">
         <v>119</v>
@@ -10027,7 +10023,7 @@
       </c>
       <c r="E11" s="41">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>1.7899999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F11" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -10035,14 +10031,14 @@
       </c>
       <c r="G11" s="40">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41890</v>
+        <v>41906</v>
       </c>
       <c r="I11" s="34">
-        <v>0.99906975550031596</v>
+        <v>0.99876957294552227</v>
       </c>
       <c r="K11" s="92" t="s">
         <v>120</v>
@@ -10057,7 +10053,7 @@
       </c>
       <c r="E12" s="41">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>1.7699999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F12" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -10065,14 +10061,14 @@
       </c>
       <c r="G12" s="40">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41918</v>
+        <v>41936</v>
       </c>
       <c r="I12" s="34">
-        <v>0.99894262626017372</v>
+        <v>0.99856919771082242</v>
       </c>
       <c r="K12" s="92" t="s">
         <v>121</v>
@@ -10087,7 +10083,7 @@
       </c>
       <c r="E13" s="41">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>1.7599999999999998E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F13" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10095,14 +10091,14 @@
       </c>
       <c r="G13" s="40">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>41949</v>
+        <v>41967</v>
       </c>
       <c r="I13" s="34">
-        <v>0.99879727546318176</v>
+        <v>0.99836901336698958</v>
       </c>
       <c r="K13" s="92" t="s">
         <v>122</v>
@@ -10117,7 +10113,7 @@
       </c>
       <c r="E14" s="41">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.7499999999999998E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F14" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10125,14 +10121,14 @@
       </c>
       <c r="G14" s="40">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>41981</v>
+        <v>41997</v>
       </c>
       <c r="I14" s="34">
-        <v>0.99864882280370604</v>
+        <v>0.99816199765888924</v>
       </c>
       <c r="K14" s="92" t="s">
         <v>123</v>
@@ -10147,7 +10143,7 @@
       </c>
       <c r="E15" s="41">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.7399999999999998E-3</v>
+        <v>2.3400000000000001E-3</v>
       </c>
       <c r="F15" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -10155,14 +10151,14 @@
       </c>
       <c r="G15" s="40">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42010</v>
+        <v>42030</v>
       </c>
       <c r="I15" s="34">
-        <v>0.99851667321467208</v>
+        <v>0.99795889176046026</v>
       </c>
       <c r="K15" s="92" t="s">
         <v>124</v>
@@ -10177,7 +10173,7 @@
       </c>
       <c r="E16" s="41">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.72E-3</v>
+        <v>2.3499999999999997E-3</v>
       </c>
       <c r="F16" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -10185,14 +10181,14 @@
       </c>
       <c r="G16" s="40">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42041</v>
+        <v>42059</v>
       </c>
       <c r="I16" s="34">
-        <v>0.99838590965857021</v>
+        <v>0.99775778414690419</v>
       </c>
       <c r="K16" s="92" t="s">
         <v>125</v>
@@ -10207,7 +10203,7 @@
       </c>
       <c r="E17" s="41">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.7099999999999999E-3</v>
+        <v>2.3599999999999997E-3</v>
       </c>
       <c r="F17" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -10215,14 +10211,14 @@
       </c>
       <c r="G17" s="40">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H17" s="39">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42069</v>
+        <v>42087</v>
       </c>
       <c r="I17" s="34">
-        <v>0.99826261920788339</v>
+        <v>0.99756179263056788</v>
       </c>
       <c r="K17" s="92" t="s">
         <v>126</v>
@@ -10237,7 +10233,7 @@
       </c>
       <c r="E18" s="41">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>2.1199999999999991E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="F18" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10245,14 +10241,14 @@
       </c>
       <c r="G18" s="40">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H18" s="39">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42436</v>
+        <v>42453</v>
       </c>
       <c r="I18" s="34">
-        <v>0.99575971972651056</v>
+        <v>0.99424231634238303</v>
       </c>
       <c r="K18" s="92" t="s">
         <v>127</v>
@@ -10267,7 +10263,7 @@
       </c>
       <c r="E19" s="41">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>3.3199999999999996E-3</v>
+        <v>3.9500000000000004E-3</v>
       </c>
       <c r="F19" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10275,14 +10271,14 @@
       </c>
       <c r="G19" s="40">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H19" s="39">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42800</v>
+        <v>42818</v>
       </c>
       <c r="I19" s="34">
-        <v>0.99008449921164365</v>
+        <v>0.9878423974235202</v>
       </c>
       <c r="K19" s="92" t="s">
         <v>128</v>
@@ -10297,7 +10293,7 @@
       </c>
       <c r="E20" s="41">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>5.0799999999999994E-3</v>
+        <v>5.6599999999999992E-3</v>
       </c>
       <c r="F20" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10305,14 +10301,14 @@
       </c>
       <c r="G20" s="40">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H20" s="39">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43165</v>
+        <v>43185</v>
       </c>
       <c r="I20" s="34">
-        <v>0.97985510070638482</v>
+        <v>0.97694400640877632</v>
       </c>
       <c r="K20" s="92" t="s">
         <v>129</v>
@@ -10327,7 +10323,7 @@
       </c>
       <c r="E21" s="41">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>6.9899999999999988E-3</v>
+        <v>7.5299999999999994E-3</v>
       </c>
       <c r="F21" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10335,14 +10331,14 @@
       </c>
       <c r="G21" s="40">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H21" s="39">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43530</v>
+        <v>43549</v>
       </c>
       <c r="I21" s="34">
-        <v>0.96553878944577554</v>
+        <v>0.96206703219314671</v>
       </c>
       <c r="K21" s="92" t="s">
         <v>130</v>
@@ -10357,7 +10353,7 @@
       </c>
       <c r="E22" s="41">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>8.9500000000000014E-3</v>
+        <v>9.4400000000000005E-3</v>
       </c>
       <c r="F22" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10365,14 +10361,14 @@
       </c>
       <c r="G22" s="40">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H22" s="39">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43896</v>
+        <v>43914</v>
       </c>
       <c r="I22" s="34">
-        <v>0.94740573853736643</v>
+        <v>0.94362634088976871</v>
       </c>
       <c r="K22" s="92" t="s">
         <v>131</v>
@@ -10387,7 +10383,7 @@
       </c>
       <c r="E23" s="41">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.0840000000000001E-2</v>
+        <v>1.1300000000000001E-2</v>
       </c>
       <c r="F23" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10395,14 +10391,14 @@
       </c>
       <c r="G23" s="40">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H23" s="39">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44263</v>
+        <v>44279</v>
       </c>
       <c r="I23" s="34">
-        <v>0.92621566266352628</v>
+        <v>0.92221843808548987</v>
       </c>
       <c r="K23" s="92" t="s">
         <v>132</v>
@@ -10417,7 +10413,7 @@
       </c>
       <c r="E24" s="41">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.26E-2</v>
+        <v>1.3059999999999999E-2</v>
       </c>
       <c r="F24" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10425,14 +10421,14 @@
       </c>
       <c r="G24" s="40">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H24" s="39">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44627</v>
+        <v>44644</v>
       </c>
       <c r="I24" s="34">
-        <v>0.90290740596766461</v>
+        <v>0.8984874041362092</v>
       </c>
       <c r="K24" s="92" t="s">
         <v>133</v>
@@ -10447,7 +10443,7 @@
       </c>
       <c r="E25" s="41">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>1.4199999999999999E-2</v>
+        <v>1.4659999999999999E-2</v>
       </c>
       <c r="F25" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10455,14 +10451,14 @@
       </c>
       <c r="G25" s="40">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H25" s="39">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44991</v>
+        <v>45009</v>
       </c>
       <c r="I25" s="34">
-        <v>0.87816075906549318</v>
+        <v>0.87336000230690747</v>
       </c>
       <c r="K25" s="92" t="s">
         <v>134</v>
@@ -10477,7 +10473,7 @@
       </c>
       <c r="E26" s="41">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>1.566E-2</v>
+        <v>1.6119999999999999E-2</v>
       </c>
       <c r="F26" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10485,14 +10481,14 @@
       </c>
       <c r="G26" s="40">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H26" s="39">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>45357</v>
+        <v>45376</v>
       </c>
       <c r="I26" s="34">
-        <v>0.85230605720525277</v>
+        <v>0.84725836974120172</v>
       </c>
       <c r="K26" s="92" t="s">
         <v>135</v>
@@ -10507,7 +10503,7 @@
       </c>
       <c r="E27" s="41">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>1.8030000000000001E-2</v>
+        <v>1.8530000000000001E-2</v>
       </c>
       <c r="F27" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10515,14 +10511,14 @@
       </c>
       <c r="G27" s="40">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H27" s="39">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>46087</v>
+        <v>46105</v>
       </c>
       <c r="I27" s="34">
-        <v>0.80065619875580585</v>
+        <v>0.79453509819643386</v>
       </c>
       <c r="K27" s="92" t="s">
         <v>136</v>
@@ -10537,7 +10533,7 @@
       </c>
       <c r="E28" s="41">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.051E-2</v>
+        <v>2.1029999999999997E-2</v>
       </c>
       <c r="F28" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10545,14 +10541,14 @@
       </c>
       <c r="G28" s="40">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H28" s="39">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>47183</v>
+        <v>47203</v>
       </c>
       <c r="I28" s="34">
-        <v>0.7270763765535937</v>
+        <v>0.71960624811297991</v>
       </c>
       <c r="K28" s="92" t="s">
         <v>137</v>
@@ -10567,7 +10563,7 @@
       </c>
       <c r="E29" s="41">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.2390000000000004E-2</v>
+        <v>2.2969999999999997E-2</v>
       </c>
       <c r="F29" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10575,14 +10571,14 @@
       </c>
       <c r="G29" s="40">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H29" s="39">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>49009</v>
+        <v>49027</v>
       </c>
       <c r="I29" s="34">
-        <v>0.62764846824122722</v>
+        <v>0.61815456993042173</v>
       </c>
       <c r="K29" s="92" t="s">
         <v>138</v>
@@ -10597,7 +10593,7 @@
       </c>
       <c r="E30" s="41">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.307E-2</v>
+        <v>2.368E-2</v>
       </c>
       <c r="F30" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -10605,14 +10601,14 @@
       </c>
       <c r="G30" s="40">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H30" s="39">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>50836</v>
+        <v>50853</v>
       </c>
       <c r="I30" s="34">
-        <v>0.54949406901264486</v>
+        <v>0.53867102014549195</v>
       </c>
       <c r="K30" s="92" t="s">
         <v>139</v>
@@ -10627,7 +10623,7 @@
       </c>
       <c r="E31" s="41">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.3279999999999999E-2</v>
+        <v>2.3899999999999998E-2</v>
       </c>
       <c r="F31" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -10635,14 +10631,14 @@
       </c>
       <c r="G31" s="40">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H31" s="39">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>52663</v>
+        <v>52680</v>
       </c>
       <c r="I31" s="34">
-        <v>0.48596314736453577</v>
+        <v>0.47459956685099797</v>
       </c>
       <c r="K31" s="92" t="s">
         <v>140</v>
@@ -10657,7 +10653,7 @@
       </c>
       <c r="E32" s="41">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.3477999999999999E-2</v>
+        <v>2.4135999999999998E-2</v>
       </c>
       <c r="F32" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -10665,14 +10661,14 @@
       </c>
       <c r="G32" s="40">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H32" s="39">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>54490</v>
+        <v>54506</v>
       </c>
       <c r="I32" s="34">
-        <v>0.42860286141435094</v>
+        <v>0.41615351594573646</v>
       </c>
       <c r="K32" s="92" t="s">
         <v>141</v>
@@ -10687,7 +10683,7 @@
       </c>
       <c r="E33" s="41">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.3699999999999999E-2</v>
+        <v>2.4420000000000001E-2</v>
       </c>
       <c r="F33" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -10695,14 +10691,14 @@
       </c>
       <c r="G33" s="40">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H33" s="39">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>56314</v>
+        <v>56332</v>
       </c>
       <c r="I33" s="34">
-        <v>0.37623722738470383</v>
+        <v>0.36251636759081063</v>
       </c>
       <c r="K33" s="92" t="s">
         <v>142</v>
@@ -10717,7 +10713,7 @@
       </c>
       <c r="E34" s="41">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.3970000000000002E-2</v>
+        <v>2.4759999999999997E-2</v>
       </c>
       <c r="F34" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -10725,14 +10721,14 @@
       </c>
       <c r="G34" s="40">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H34" s="39">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>59967</v>
+        <v>59985</v>
       </c>
       <c r="I34" s="34">
-        <v>0.29069108595720217</v>
+        <v>0.27588776885579702</v>
       </c>
       <c r="K34" s="92" t="s">
         <v>143</v>
@@ -10747,7 +10743,7 @@
       </c>
       <c r="E35" s="41">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.418E-2</v>
+        <v>2.4970000000000003E-2</v>
       </c>
       <c r="F35" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -10755,14 +10751,14 @@
       </c>
       <c r="G35" s="40">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41704</v>
+        <v>41722</v>
       </c>
       <c r="H35" s="39">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>63619</v>
+        <v>63639</v>
       </c>
       <c r="I35" s="34">
-        <v>0.22347000001388923</v>
+        <v>0.2099941941173552</v>
       </c>
       <c r="K35" s="43" t="s">
         <v>144</v>
@@ -13065,24 +13061,24 @@
       <c r="B3" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="187" t="s">
+      <c r="C3" s="178" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="187">
+      <c r="D3" s="178">
         <f>_xll.qlInterestRateIndexFixingDays($F$1,Trigger)</f>
         <v>2</v>
       </c>
-      <c r="E3" s="187" t="str">
+      <c r="E3" s="178" t="str">
         <f>_xll.qlIndexFixingCalendar($F$1,Trigger)</f>
         <v>TARGET</v>
       </c>
-      <c r="F3" s="187" t="s">
+      <c r="F3" s="178" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="187" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="187" t="str">
+      <c r="G3" s="178" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="178" t="str">
         <f>_xll.qlInterestRateIndexDayCounter($F$1,Trigger)</f>
         <v>Actual/360</v>
       </c>
@@ -13096,7 +13092,7 @@
       </c>
       <c r="K3" s="100" t="str">
         <f>_xll.qlDepositRateHelper2(J3,I3,C3,D3,E3,F3,G3,H3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_SND#0009</v>
+        <v>EUR_YC1MRH_SND#0000</v>
       </c>
       <c r="L3" s="99" t="str">
         <f>_xll.ohRangeRetrieveError(K3)</f>
@@ -13109,24 +13105,24 @@
       <c r="B4" s="104" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="187" t="s">
+      <c r="C4" s="178" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="187">
+      <c r="D4" s="178">
         <f>_xll.qlInterestRateIndexFixingDays($F$1,Trigger)</f>
         <v>2</v>
       </c>
-      <c r="E4" s="187" t="str">
+      <c r="E4" s="178" t="str">
         <f>_xll.qlIndexFixingCalendar($F$1,Trigger)</f>
         <v>TARGET</v>
       </c>
-      <c r="F4" s="187" t="s">
+      <c r="F4" s="178" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="187" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="187" t="str">
+      <c r="G4" s="178" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="178" t="str">
         <f>_xll.qlInterestRateIndexDayCounter($F$1,Trigger)</f>
         <v>Actual/360</v>
       </c>
@@ -13140,7 +13136,7 @@
       </c>
       <c r="K4" s="100" t="str">
         <f>_xll.qlDepositRateHelper2(J4,I4,C4,D4,E4,F4,G4,H4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_SWD#0008</v>
+        <v>EUR_YC1MRH_SWD#0000</v>
       </c>
       <c r="L4" s="99" t="str">
         <f>_xll.ohRangeRetrieveError(K4)</f>
@@ -13153,24 +13149,24 @@
       <c r="B5" s="104" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="187" t="s">
+      <c r="C5" s="178" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="187">
+      <c r="D5" s="178">
         <f>_xll.qlInterestRateIndexFixingDays($F$1,Trigger)</f>
         <v>2</v>
       </c>
-      <c r="E5" s="187" t="str">
+      <c r="E5" s="178" t="str">
         <f>_xll.qlIndexFixingCalendar($F$1,Trigger)</f>
         <v>TARGET</v>
       </c>
-      <c r="F5" s="187" t="s">
+      <c r="F5" s="178" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="187" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="187" t="str">
+      <c r="G5" s="178" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="178" t="str">
         <f>_xll.qlInterestRateIndexDayCounter($F$1,Trigger)</f>
         <v>Actual/360</v>
       </c>
@@ -13184,7 +13180,7 @@
       </c>
       <c r="K5" s="100" t="str">
         <f>_xll.qlDepositRateHelper2(J5,I5,C5,D5,E5,F5,G5,H5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2WD#0008</v>
+        <v>EUR_YC1MRH_2WD#0000</v>
       </c>
       <c r="L5" s="99" t="str">
         <f>_xll.ohRangeRetrieveError(K5)</f>
@@ -13197,24 +13193,24 @@
       <c r="B6" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="187" t="s">
+      <c r="C6" s="178" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="187">
+      <c r="D6" s="178">
         <f>_xll.qlInterestRateIndexFixingDays($F$1,Trigger)</f>
         <v>2</v>
       </c>
-      <c r="E6" s="187" t="str">
+      <c r="E6" s="178" t="str">
         <f>_xll.qlIndexFixingCalendar($F$1,Trigger)</f>
         <v>TARGET</v>
       </c>
-      <c r="F6" s="187" t="s">
+      <c r="F6" s="178" t="s">
         <v>202</v>
       </c>
-      <c r="G6" s="187" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="187" t="str">
+      <c r="G6" s="178" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="178" t="str">
         <f>_xll.qlInterestRateIndexDayCounter($F$1,Trigger)</f>
         <v>Actual/360</v>
       </c>
@@ -13228,7 +13224,7 @@
       </c>
       <c r="K6" s="100" t="str">
         <f>_xll.qlDepositRateHelper2(J6,I6,C6,D6,E6,F6,G6,H6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3WD#0001</v>
+        <v>EUR_YC1MRH_3WD#0000</v>
       </c>
       <c r="L6" s="99" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -13241,26 +13237,26 @@
       <c r="B7" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="187" t="s">
+      <c r="C7" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="187">
+      <c r="D7" s="178">
         <f>_xll.qlInterestRateIndexFixingDays($F$1,Trigger)</f>
         <v>2</v>
       </c>
-      <c r="E7" s="187" t="str">
+      <c r="E7" s="178" t="str">
         <f>_xll.qlIndexFixingCalendar($F$1,Trigger)</f>
         <v>TARGET</v>
       </c>
-      <c r="F7" s="187" t="str">
+      <c r="F7" s="178" t="str">
         <f>_xll.qlIborIndexBusinessDayConv($F$1,Trigger)</f>
         <v>Modified Following</v>
       </c>
-      <c r="G7" s="187" t="b">
+      <c r="G7" s="178" t="b">
         <f>_xll.qlIborIndexEndOfMonth($F$1,Trigger)</f>
         <v>1</v>
       </c>
-      <c r="H7" s="187" t="str">
+      <c r="H7" s="178" t="str">
         <f>_xll.qlInterestRateIndexDayCounter($F$1,Trigger)</f>
         <v>Actual/360</v>
       </c>
@@ -13274,7 +13270,7 @@
       </c>
       <c r="K7" s="100" t="str">
         <f>_xll.qlDepositRateHelper2(J7,I7,C7,D7,E7,F7,G7,H7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_1MD#0011</v>
+        <v>EUR_YC1MRH_1MD#0000</v>
       </c>
       <c r="L7" s="99" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -13430,7 +13426,7 @@
       </c>
       <c r="L4" s="146" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1MRH_xX1S_ibor1M#0001</v>
+        <v>EUR_YC1MRH_xX1S_ibor1M#0000</v>
       </c>
       <c r="M4" s="145" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -13491,7 +13487,7 @@
       </c>
       <c r="L6" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2X1S#0001</v>
+        <v>EUR_YC1MRH_2X1S#0000</v>
       </c>
       <c r="M6" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -13536,7 +13532,7 @@
       </c>
       <c r="L7" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3X1S#0001</v>
+        <v>EUR_YC1MRH_3X1S#0000</v>
       </c>
       <c r="M7" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -13581,7 +13577,7 @@
       </c>
       <c r="L8" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_4X1S#0001</v>
+        <v>EUR_YC1MRH_4X1S#0000</v>
       </c>
       <c r="M8" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -13626,7 +13622,7 @@
       </c>
       <c r="L9" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_5X1S#0001</v>
+        <v>EUR_YC1MRH_5X1S#0000</v>
       </c>
       <c r="M9" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -13671,7 +13667,7 @@
       </c>
       <c r="L10" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_6X1S#0001</v>
+        <v>EUR_YC1MRH_6X1S#0000</v>
       </c>
       <c r="M10" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -13716,7 +13712,7 @@
       </c>
       <c r="L11" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_7X1S#0001</v>
+        <v>EUR_YC1MRH_7X1S#0000</v>
       </c>
       <c r="M11" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -13761,7 +13757,7 @@
       </c>
       <c r="L12" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_8X1S#0001</v>
+        <v>EUR_YC1MRH_8X1S#0000</v>
       </c>
       <c r="M12" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -13806,7 +13802,7 @@
       </c>
       <c r="L13" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_9X1S#0001</v>
+        <v>EUR_YC1MRH_9X1S#0000</v>
       </c>
       <c r="M13" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -13851,7 +13847,7 @@
       </c>
       <c r="L14" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_10X1S#0001</v>
+        <v>EUR_YC1MRH_10X1S#0000</v>
       </c>
       <c r="M14" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -13896,7 +13892,7 @@
       </c>
       <c r="L15" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_11X1S#0001</v>
+        <v>EUR_YC1MRH_11X1S#0000</v>
       </c>
       <c r="M15" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -13941,7 +13937,7 @@
       </c>
       <c r="L16" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_12X1S#0001</v>
+        <v>EUR_YC1MRH_12X1S#0000</v>
       </c>
       <c r="M16" s="107" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -14124,7 +14120,7 @@
       </c>
       <c r="L4" s="146" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1MRH_AB1EBASIS_ibor1M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS_ibor1M#0000</v>
       </c>
       <c r="M4" s="145" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -14188,7 +14184,7 @@
       </c>
       <c r="L6" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS1Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS1Y#0000</v>
       </c>
       <c r="M6" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -14237,7 +14233,7 @@
       </c>
       <c r="L7" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS15M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15M#0000</v>
       </c>
       <c r="M7" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -14286,7 +14282,7 @@
       </c>
       <c r="L8" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS18M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18M#0000</v>
       </c>
       <c r="M8" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -14335,7 +14331,7 @@
       </c>
       <c r="L9" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS21M#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21M#0000</v>
       </c>
       <c r="M9" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -14384,7 +14380,7 @@
       </c>
       <c r="L10" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS2Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS2Y#0000</v>
       </c>
       <c r="M10" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -14442,7 +14438,7 @@
       </c>
       <c r="L11" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS3Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS3Y#0000</v>
       </c>
       <c r="M11" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -14500,7 +14496,7 @@
       </c>
       <c r="L12" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS4Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS4Y#0000</v>
       </c>
       <c r="M12" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -14558,7 +14554,7 @@
       </c>
       <c r="L13" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS5Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS5Y#0000</v>
       </c>
       <c r="M13" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -14616,7 +14612,7 @@
       </c>
       <c r="L14" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS6Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS6Y#0000</v>
       </c>
       <c r="M14" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -14674,7 +14670,7 @@
       </c>
       <c r="L15" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS7Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS7Y#0000</v>
       </c>
       <c r="M15" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -14726,7 +14722,7 @@
       </c>
       <c r="L16" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS8Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS8Y#0000</v>
       </c>
       <c r="M16" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -14775,7 +14771,7 @@
       </c>
       <c r="L17" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS9Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS9Y#0000</v>
       </c>
       <c r="M17" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -14824,7 +14820,7 @@
       </c>
       <c r="L18" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS10Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS10Y#0000</v>
       </c>
       <c r="M18" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -14873,7 +14869,7 @@
       </c>
       <c r="L19" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS11Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS11Y#0000</v>
       </c>
       <c r="M19" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -14922,7 +14918,7 @@
       </c>
       <c r="L20" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS12Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS12Y#0000</v>
       </c>
       <c r="M20" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -14971,7 +14967,7 @@
       </c>
       <c r="L21" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS13Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS13Y#0000</v>
       </c>
       <c r="M21" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -15020,7 +15016,7 @@
       </c>
       <c r="L22" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS14Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS14Y#0000</v>
       </c>
       <c r="M22" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -15069,7 +15065,7 @@
       </c>
       <c r="L23" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS15Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS15Y#0000</v>
       </c>
       <c r="M23" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -15118,7 +15114,7 @@
       </c>
       <c r="L24" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS16Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS16Y#0000</v>
       </c>
       <c r="M24" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -15167,7 +15163,7 @@
       </c>
       <c r="L25" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS17Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS17Y#0000</v>
       </c>
       <c r="M25" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -15216,7 +15212,7 @@
       </c>
       <c r="L26" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS18Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS18Y#0000</v>
       </c>
       <c r="M26" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -15265,7 +15261,7 @@
       </c>
       <c r="L27" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS19Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS19Y#0000</v>
       </c>
       <c r="M27" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -15314,7 +15310,7 @@
       </c>
       <c r="L28" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS20Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS20Y#0000</v>
       </c>
       <c r="M28" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -15363,7 +15359,7 @@
       </c>
       <c r="L29" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS21Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS21Y#0000</v>
       </c>
       <c r="M29" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -15412,7 +15408,7 @@
       </c>
       <c r="L30" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS22Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS22Y#0000</v>
       </c>
       <c r="M30" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -15461,7 +15457,7 @@
       </c>
       <c r="L31" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS23Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS23Y#0000</v>
       </c>
       <c r="M31" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -15510,7 +15506,7 @@
       </c>
       <c r="L32" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS24Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS24Y#0000</v>
       </c>
       <c r="M32" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -15559,7 +15555,7 @@
       </c>
       <c r="L33" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS25Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS25Y#0000</v>
       </c>
       <c r="M33" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -15608,7 +15604,7 @@
       </c>
       <c r="L34" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS26Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS26Y#0000</v>
       </c>
       <c r="M34" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -15657,7 +15653,7 @@
       </c>
       <c r="L35" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS27Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS27Y#0000</v>
       </c>
       <c r="M35" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -15706,7 +15702,7 @@
       </c>
       <c r="L36" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS28Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS28Y#0000</v>
       </c>
       <c r="M36" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -15755,7 +15751,7 @@
       </c>
       <c r="L37" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS29Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS29Y#0000</v>
       </c>
       <c r="M37" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -15804,7 +15800,7 @@
       </c>
       <c r="L38" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS30Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS30Y#0000</v>
       </c>
       <c r="M38" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -15853,7 +15849,7 @@
       </c>
       <c r="L39" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS35Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS35Y#0000</v>
       </c>
       <c r="M39" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -15902,7 +15898,7 @@
       </c>
       <c r="L40" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS40Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS40Y#0000</v>
       </c>
       <c r="M40" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -15951,7 +15947,7 @@
       </c>
       <c r="L41" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS50Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS50Y#0000</v>
       </c>
       <c r="M41" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -16000,7 +15996,7 @@
       </c>
       <c r="L42" s="138" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_AB1EBASIS60Y#0001</v>
+        <v>EUR_YC1MRH_AB1EBASIS60Y#0000</v>
       </c>
       <c r="M42" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>

<commit_message>
used MidSafe wherever appropriate, removed usage of non quoted basis, removed useless interpolations
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2082,8 +2082,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2105,7 @@
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="165" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Mar  3 2014 10:58:57</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 18 2014 11:20:01</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D14" s="81" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC1M#0001</v>
+        <v>_EURYC1M#0002</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -2504,7 +2504,7 @@
       <c r="B27" s="59"/>
       <c r="C27" s="63">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41739</v>
+        <v>41752</v>
       </c>
       <c r="D27" s="62">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2517,11 +2517,11 @@
       <c r="B28" s="59"/>
       <c r="C28" s="61">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>63654</v>
+        <v>63668</v>
       </c>
       <c r="D28" s="60">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.2203744773058621</v>
+        <v>0.22762105274163486</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="57"/>
@@ -2602,7 +2602,7 @@
   <dimension ref="A1:N167"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="F2" s="13">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>2.7929999999999999E-3</v>
+        <v>2.6749999999999999E-3</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="12" t="b">
@@ -2682,11 +2682,11 @@
       </c>
       <c r="K2" s="11">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L2" s="10">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41740</v>
+        <v>41754</v>
       </c>
       <c r="M2" s="1">
         <v>30</v>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="F3" s="13">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>2.385E-3</v>
+        <v>2.5040000000000001E-3</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="12" t="b">
@@ -2721,11 +2721,11 @@
       </c>
       <c r="K3" s="11">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L3" s="10">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41746</v>
+        <v>41761</v>
       </c>
       <c r="M3" s="1">
         <v>40</v>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>2.552E-3</v>
+        <v>2.575E-3</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="12" t="b">
@@ -2760,11 +2760,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41753</v>
+        <v>41767</v>
       </c>
       <c r="M4" s="1">
         <v>50</v>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="F5" s="13">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>2.5820000000000001E-3</v>
+        <v>2.4989999999999999E-3</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="12" t="b">
@@ -2799,11 +2799,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41761</v>
+        <v>41774</v>
       </c>
       <c r="M5" s="1">
         <v>60</v>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="F6" s="13">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>2.5100000000000001E-3</v>
+        <v>2.4599999999999999E-3</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="12" t="b">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41771</v>
+        <v>41785</v>
       </c>
       <c r="M6" s="1">
         <v>70</v>
@@ -3856,11 +3856,11 @@
       </c>
       <c r="D34" s="14" t="str">
         <f t="array" ref="D34:D75">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A34:$A75)</f>
-        <v>J4</v>
+        <v>K4</v>
       </c>
       <c r="E34" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MJ4</v>
+        <v>EUR_YC1MRH_FUT1MK4</v>
       </c>
       <c r="F34" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E34,Trigger)</f>
@@ -3898,11 +3898,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D35" s="14" t="str">
-        <v>K4</v>
+        <v>M4</v>
       </c>
       <c r="E35" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MK4</v>
+        <v>EUR_YC1MRH_FUT1MM4</v>
       </c>
       <c r="F35" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
@@ -3940,11 +3940,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D36" s="14" t="str">
-        <v>M4</v>
+        <v>N4</v>
       </c>
       <c r="E36" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MM4</v>
+        <v>EUR_YC1MRH_FUT1MN4</v>
       </c>
       <c r="F36" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -3982,11 +3982,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D37" s="14" t="str">
-        <v>N4</v>
+        <v>Q4</v>
       </c>
       <c r="E37" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MN4</v>
+        <v>EUR_YC1MRH_FUT1MQ4</v>
       </c>
       <c r="F37" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4024,11 +4024,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D38" s="14" t="str">
-        <v>Q4</v>
+        <v>U4</v>
       </c>
       <c r="E38" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MQ4</v>
+        <v>EUR_YC1MRH_FUT1MU4</v>
       </c>
       <c r="F38" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4066,11 +4066,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D39" s="14" t="str">
-        <v>U4</v>
+        <v>V4</v>
       </c>
       <c r="E39" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MU4</v>
+        <v>EUR_YC1MRH_FUT1MV4</v>
       </c>
       <c r="F39" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4108,11 +4108,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D40" s="14" t="str">
-        <v>V4</v>
+        <v>X4</v>
       </c>
       <c r="E40" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MV4</v>
+        <v>EUR_YC1MRH_FUT1MX4</v>
       </c>
       <c r="F40" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4150,11 +4150,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D41" s="14" t="str">
-        <v>X4</v>
+        <v>Z4</v>
       </c>
       <c r="E41" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MX4</v>
+        <v>EUR_YC1MRH_FUT1MZ4</v>
       </c>
       <c r="F41" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4192,11 +4192,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D42" s="14" t="str">
-        <v>Z4</v>
+        <v>F5</v>
       </c>
       <c r="E42" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MZ4</v>
+        <v>EUR_YC1MRH_FUT1MF5</v>
       </c>
       <c r="F42" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4234,11 +4234,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D43" s="14" t="str">
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E43" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MF5</v>
+        <v>EUR_YC1MRH_FUT1MG5</v>
       </c>
       <c r="F43" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4276,11 +4276,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D44" s="14" t="str">
-        <v>G5</v>
+        <v>H5</v>
       </c>
       <c r="E44" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MG5</v>
+        <v>EUR_YC1MRH_FUT1MH5</v>
       </c>
       <c r="F44" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4318,11 +4318,11 @@
         <v>FUT1M</v>
       </c>
       <c r="D45" s="14" t="str">
-        <v>H5</v>
+        <v>J5</v>
       </c>
       <c r="E45" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1MRH_FUT1MH5</v>
+        <v>EUR_YC1MRH_FUT1MJ5</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="F76" s="20">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>2.48E-3</v>
+        <v>2.4199999999999998E-3</v>
       </c>
       <c r="G76" s="20">
         <f>_xll.qlSwapRateHelperSpread($E76,Trigger)</f>
@@ -5642,11 +5642,11 @@
       </c>
       <c r="K76" s="18">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L76" s="17">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>41800</v>
+        <v>41814</v>
       </c>
       <c r="M76" s="22"/>
     </row>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="F77" s="13">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
-        <v>2.3999999999999998E-3</v>
+        <v>2.33E-3</v>
       </c>
       <c r="G77" s="13">
         <f>_xll.qlSwapRateHelperSpread($E77,Trigger)</f>
@@ -5681,11 +5681,11 @@
       </c>
       <c r="K77" s="11">
         <f>_xll.qlRateHelperEarliestDate($E77,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L77" s="10">
         <f>_xll.qlRateHelperLatestDate($E77,Trigger)</f>
-        <v>41830</v>
+        <v>41844</v>
       </c>
       <c r="M77" s="25"/>
     </row>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="F78" s="13">
         <f>_xll.qlRateHelperQuoteValue($E78,Trigger)</f>
-        <v>2.33E-3</v>
+        <v>2.2599999999999999E-3</v>
       </c>
       <c r="G78" s="13">
         <f>_xll.qlSwapRateHelperSpread($E78,Trigger)</f>
@@ -5720,11 +5720,11 @@
       </c>
       <c r="K78" s="11">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L78" s="10">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>41862</v>
+        <v>41876</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="F79" s="13">
         <f>_xll.qlRateHelperQuoteValue($E79,Trigger)</f>
-        <v>2.2799999999999999E-3</v>
+        <v>2.2100000000000002E-3</v>
       </c>
       <c r="G79" s="13">
         <f>_xll.qlSwapRateHelperSpread($E79,Trigger)</f>
@@ -5758,11 +5758,11 @@
       </c>
       <c r="K79" s="11">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L79" s="10">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>41892</v>
+        <v>41906</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="F80" s="13">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
-        <v>2.2300000000000002E-3</v>
+        <v>2.16E-3</v>
       </c>
       <c r="G80" s="13">
         <f>_xll.qlSwapRateHelperSpread($E80,Trigger)</f>
@@ -5796,11 +5796,11 @@
       </c>
       <c r="K80" s="11">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L80" s="10">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>41922</v>
+        <v>41936</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
@@ -5817,7 +5817,7 @@
       </c>
       <c r="F81" s="13">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
-        <v>2.1800000000000001E-3</v>
+        <v>2.1199999999999999E-3</v>
       </c>
       <c r="G81" s="13">
         <f>_xll.qlSwapRateHelperSpread($E81,Trigger)</f>
@@ -5834,11 +5834,11 @@
       </c>
       <c r="K81" s="11">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L81" s="10">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>41953</v>
+        <v>41967</v>
       </c>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.2">
@@ -5855,7 +5855,7 @@
       </c>
       <c r="F82" s="13">
         <f>_xll.qlRateHelperQuoteValue($E82,Trigger)</f>
-        <v>2.14E-3</v>
+        <v>2.0800000000000003E-3</v>
       </c>
       <c r="G82" s="13">
         <f>_xll.qlSwapRateHelperSpread($E82,Trigger)</f>
@@ -5872,11 +5872,11 @@
       </c>
       <c r="K82" s="11">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L82" s="10">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>41983</v>
+        <v>41997</v>
       </c>
     </row>
     <row r="83" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="F83" s="13">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
-        <v>2.1199999999999999E-3</v>
+        <v>2.0500000000000002E-3</v>
       </c>
       <c r="G83" s="13">
         <f>_xll.qlSwapRateHelperSpread($E83,Trigger)</f>
@@ -5910,11 +5910,11 @@
       </c>
       <c r="K83" s="11">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L83" s="10">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>42016</v>
+        <v>42030</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="F84" s="13">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
-        <v>2.0900000000000003E-3</v>
+        <v>2.0300000000000001E-3</v>
       </c>
       <c r="G84" s="13">
         <f>_xll.qlSwapRateHelperSpread($E84,Trigger)</f>
@@ -5948,11 +5948,11 @@
       </c>
       <c r="K84" s="11">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L84" s="10">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>42045</v>
+        <v>42059</v>
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.2">
@@ -5969,7 +5969,7 @@
       </c>
       <c r="F85" s="13">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
-        <v>2.0600000000000002E-3</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="G85" s="13">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
@@ -5986,11 +5986,11 @@
       </c>
       <c r="K85" s="11">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L85" s="10">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>42073</v>
+        <v>42087</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
@@ -6007,7 +6007,7 @@
       </c>
       <c r="F86" s="6">
         <f>_xll.qlRateHelperQuoteValue($E86,Trigger)</f>
-        <v>2.0500000000000002E-3</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="G86" s="6">
         <f>_xll.qlSwapRateHelperSpread($E86,Trigger)</f>
@@ -6024,11 +6024,11 @@
       </c>
       <c r="K86" s="4">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L86" s="3">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>42104</v>
+        <v>42118</v>
       </c>
     </row>
     <row r="87" spans="2:14" hidden="1" x14ac:dyDescent="0.2">
@@ -8017,7 +8017,7 @@
       </c>
       <c r="F131" s="20">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
-        <v>2.0700000000000002E-3</v>
+        <v>2.0400000000000001E-3</v>
       </c>
       <c r="G131" s="20">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
@@ -8034,11 +8034,11 @@
       </c>
       <c r="K131" s="18">
         <f>_xll.qlRateHelperEarliestDate($E131,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L131" s="17">
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
-        <v>42104</v>
+        <v>42118</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
@@ -8057,9 +8057,9 @@
         <f>'1M_SwapsFromBasis'!L7</f>
         <v>EUR_YC1MRH_AB1EBASIS15M#0001</v>
       </c>
-      <c r="F132" s="13">
+      <c r="F132" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E132,Trigger)</f>
-        <v>1.856E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G132" s="13">
         <f>_xll.qlSwapRateHelperSpread($E132,Trigger)</f>
@@ -8076,11 +8076,11 @@
       </c>
       <c r="K132" s="11">
         <f>_xll.qlRateHelperEarliestDate($E132,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L132" s="10">
         <f>_xll.qlRateHelperLatestDate($E132,Trigger)</f>
-        <v>42195</v>
+        <v>42209</v>
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.2">
@@ -8099,9 +8099,9 @@
         <f>'1M_SwapsFromBasis'!L8</f>
         <v>EUR_YC1MRH_AB1EBASIS18M#0001</v>
       </c>
-      <c r="F133" s="13">
+      <c r="F133" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E133,Trigger)</f>
-        <v>2.1809999999999998E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G133" s="13">
         <f>_xll.qlSwapRateHelperSpread($E133,Trigger)</f>
@@ -8118,11 +8118,11 @@
       </c>
       <c r="K133" s="11">
         <f>_xll.qlRateHelperEarliestDate($E133,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L133" s="10">
         <f>_xll.qlRateHelperLatestDate($E133,Trigger)</f>
-        <v>42289</v>
+        <v>42303</v>
       </c>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.2">
@@ -8141,9 +8141,9 @@
         <f>'1M_SwapsFromBasis'!L9</f>
         <v>EUR_YC1MRH_AB1EBASIS21M#0001</v>
       </c>
-      <c r="F134" s="13">
+      <c r="F134" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E134,Trigger)</f>
-        <v>2.1329999999999999E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G134" s="13">
         <f>_xll.qlSwapRateHelperSpread($E134,Trigger)</f>
@@ -8160,11 +8160,11 @@
       </c>
       <c r="K134" s="11">
         <f>_xll.qlRateHelperEarliestDate($E134,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L134" s="10">
         <f>_xll.qlRateHelperLatestDate($E134,Trigger)</f>
-        <v>42380</v>
+        <v>42394</v>
       </c>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.2">
@@ -8185,7 +8185,7 @@
       </c>
       <c r="F135" s="13">
         <f>_xll.qlRateHelperQuoteValue($E135,Trigger)</f>
-        <v>2.4399999999999999E-3</v>
+        <v>2.4299999999999999E-3</v>
       </c>
       <c r="G135" s="13">
         <f>_xll.qlSwapRateHelperSpread($E135,Trigger)</f>
@@ -8202,11 +8202,11 @@
       </c>
       <c r="K135" s="11">
         <f>_xll.qlRateHelperEarliestDate($E135,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L135" s="10">
         <f>_xll.qlRateHelperLatestDate($E135,Trigger)</f>
-        <v>42471</v>
+        <v>42485</v>
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.2">
@@ -8227,7 +8227,7 @@
       </c>
       <c r="F136" s="13">
         <f>_xll.qlRateHelperQuoteValue($E136,Trigger)</f>
-        <v>3.4199999999999999E-3</v>
+        <v>3.4399999999999995E-3</v>
       </c>
       <c r="G136" s="13">
         <f>_xll.qlSwapRateHelperSpread($E136,Trigger)</f>
@@ -8244,11 +8244,11 @@
       </c>
       <c r="K136" s="11">
         <f>_xll.qlRateHelperEarliestDate($E136,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L136" s="10">
         <f>_xll.qlRateHelperLatestDate($E136,Trigger)</f>
-        <v>42835</v>
+        <v>42849</v>
       </c>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.2">
@@ -8269,7 +8269,7 @@
       </c>
       <c r="F137" s="13">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>4.9399999999999999E-3</v>
+        <v>5.0400000000000002E-3</v>
       </c>
       <c r="G137" s="13">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -8286,11 +8286,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>43200</v>
+        <v>43214</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8311,7 +8311,7 @@
       </c>
       <c r="F138" s="13">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>6.6699999999999997E-3</v>
+        <v>6.8400000000000006E-3</v>
       </c>
       <c r="G138" s="13">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -8328,11 +8328,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>43565</v>
+        <v>43579</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8353,7 +8353,7 @@
       </c>
       <c r="F139" s="13">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>8.5100000000000019E-3</v>
+        <v>8.6599999999999993E-3</v>
       </c>
       <c r="G139" s="13">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -8370,11 +8370,11 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>43935</v>
+        <v>43945</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
@@ -8395,7 +8395,7 @@
       </c>
       <c r="F140" s="13">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>1.03E-2</v>
+        <v>1.042E-2</v>
       </c>
       <c r="G140" s="13">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -8412,11 +8412,11 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>44298</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
@@ -8437,7 +8437,7 @@
       </c>
       <c r="F141" s="13">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>1.2019999999999999E-2</v>
+        <v>1.2100000000000001E-2</v>
       </c>
       <c r="G141" s="13">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -8454,11 +8454,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>44662</v>
+        <v>44676</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8479,7 +8479,7 @@
       </c>
       <c r="F142" s="13">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>1.359E-2</v>
+        <v>1.3650000000000001E-2</v>
       </c>
       <c r="G142" s="13">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -8496,11 +8496,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>45027</v>
+        <v>45040</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8521,7 +8521,7 @@
       </c>
       <c r="F143" s="13">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>1.5010000000000001E-2</v>
+        <v>1.506E-2</v>
       </c>
       <c r="G143" s="13">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -8538,11 +8538,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>45392</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="F144" s="13">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>1.6309999999999998E-2</v>
+        <v>1.6310000000000002E-2</v>
       </c>
       <c r="G144" s="13">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -8580,11 +8580,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>45757</v>
+        <v>45771</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8605,7 +8605,7 @@
       </c>
       <c r="F145" s="13">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>1.7449999999999997E-2</v>
+        <v>1.7419999999999998E-2</v>
       </c>
       <c r="G145" s="13">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -8622,11 +8622,11 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>46122</v>
+        <v>46136</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
@@ -8645,9 +8645,9 @@
         <f>'1M_SwapsFromBasis'!L21</f>
         <v>EUR_YC1MRH_AB1EBASIS13Y#0001</v>
       </c>
-      <c r="F146" s="13">
+      <c r="F146" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>1.8442999999999998E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G146" s="13">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -8664,11 +8664,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>46489</v>
+        <v>46503</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8687,9 +8687,9 @@
         <f>'1M_SwapsFromBasis'!L22</f>
         <v>EUR_YC1MRH_AB1EBASIS14Y#0001</v>
       </c>
-      <c r="F147" s="13">
+      <c r="F147" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>1.9307999999999999E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G147" s="13">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -8706,11 +8706,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46853</v>
+        <v>46867</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="F148" s="13">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>2.0029999999999999E-2</v>
+        <v>1.993E-2</v>
       </c>
       <c r="G148" s="13">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -8748,11 +8748,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>47218</v>
+        <v>47232</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8771,9 +8771,9 @@
         <f>'1M_SwapsFromBasis'!L24</f>
         <v>EUR_YC1MRH_AB1EBASIS16Y#0001</v>
       </c>
-      <c r="F149" s="13">
+      <c r="F149" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>2.0635999999999998E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G149" s="13">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -8790,11 +8790,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>47583</v>
+        <v>47597</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8813,9 +8813,9 @@
         <f>'1M_SwapsFromBasis'!L25</f>
         <v>EUR_YC1MRH_AB1EBASIS17Y#0001</v>
       </c>
-      <c r="F150" s="13">
+      <c r="F150" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>2.1125999999999999E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G150" s="13">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -8832,11 +8832,11 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>47948</v>
+        <v>47962</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
@@ -8855,9 +8855,9 @@
         <f>'1M_SwapsFromBasis'!L26</f>
         <v>EUR_YC1MRH_AB1EBASIS18Y#0001</v>
       </c>
-      <c r="F151" s="13">
+      <c r="F151" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>2.1540000000000004E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G151" s="13">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -8874,11 +8874,11 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>48316</v>
+        <v>48330</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
@@ -8897,9 +8897,9 @@
         <f>'1M_SwapsFromBasis'!L27</f>
         <v>EUR_YC1MRH_AB1EBASIS19Y#0001</v>
       </c>
-      <c r="F152" s="13">
+      <c r="F152" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>2.1867999999999999E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G152" s="13">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -8916,11 +8916,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>48680</v>
+        <v>48694</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="F153" s="13">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>2.214E-2</v>
+        <v>2.1920000000000002E-2</v>
       </c>
       <c r="G153" s="13">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -8958,11 +8958,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>49045</v>
+        <v>49058</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -8981,9 +8981,9 @@
         <f>'1M_SwapsFromBasis'!L29</f>
         <v>EUR_YC1MRH_AB1EBASIS21Y#0001</v>
       </c>
-      <c r="F154" s="13">
+      <c r="F154" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>2.2366999999999998E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G154" s="13">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -9000,11 +9000,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>49409</v>
+        <v>49423</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9023,9 +9023,9 @@
         <f>'1M_SwapsFromBasis'!L30</f>
         <v>EUR_YC1MRH_AB1EBASIS22Y#0001</v>
       </c>
-      <c r="F155" s="13">
+      <c r="F155" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>2.256E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G155" s="13">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -9042,11 +9042,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>49775</v>
+        <v>49789</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9065,9 +9065,9 @@
         <f>'1M_SwapsFromBasis'!L31</f>
         <v>EUR_YC1MRH_AB1EBASIS23Y#0001</v>
       </c>
-      <c r="F156" s="13">
+      <c r="F156" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>2.2709000000000003E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G156" s="13">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -9084,11 +9084,11 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>50140</v>
+        <v>50154</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
@@ -9107,9 +9107,9 @@
         <f>'1M_SwapsFromBasis'!L32</f>
         <v>EUR_YC1MRH_AB1EBASIS24Y#0001</v>
       </c>
-      <c r="F157" s="13">
+      <c r="F157" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>2.2836000000000002E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G157" s="13">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -9126,11 +9126,11 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>50507</v>
+        <v>50522</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
@@ -9151,7 +9151,7 @@
       </c>
       <c r="F158" s="13">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>2.2940000000000002E-2</v>
+        <v>2.265E-2</v>
       </c>
       <c r="G158" s="13">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -9168,11 +9168,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50872</v>
+        <v>50885</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9191,9 +9191,9 @@
         <f>'1M_SwapsFromBasis'!L34</f>
         <v>EUR_YC1MRH_AB1EBASIS26Y#0001</v>
       </c>
-      <c r="F159" s="13">
+      <c r="F159" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>2.3023000000000002E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G159" s="13">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -9210,11 +9210,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>51236</v>
+        <v>51250</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9233,9 +9233,9 @@
         <f>'1M_SwapsFromBasis'!L35</f>
         <v>EUR_YC1MRH_AB1EBASIS27Y#0001</v>
       </c>
-      <c r="F160" s="13">
+      <c r="F160" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>2.3094E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G160" s="13">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -9252,11 +9252,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>51601</v>
+        <v>51615</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9275,9 +9275,9 @@
         <f>'1M_SwapsFromBasis'!L36</f>
         <v>EUR_YC1MRH_AB1EBASIS28Y#0001</v>
       </c>
-      <c r="F161" s="13">
+      <c r="F161" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>2.3154000000000001E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G161" s="13">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -9294,11 +9294,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>51966</v>
+        <v>51980</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9317,9 +9317,9 @@
         <f>'1M_SwapsFromBasis'!L37</f>
         <v>EUR_YC1MRH_AB1EBASIS29Y#0001</v>
       </c>
-      <c r="F162" s="13">
+      <c r="F162" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>2.3213000000000001E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G162" s="13">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -9336,11 +9336,11 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>52331</v>
+        <v>52345</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.2">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="F163" s="13">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>2.3259999999999999E-2</v>
+        <v>2.2910000000000003E-2</v>
       </c>
       <c r="G163" s="13">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -9378,11 +9378,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>52698</v>
+        <v>52712</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9401,16 +9401,16 @@
         <f>'1M_SwapsFromBasis'!L39</f>
         <v>EUR_YC1MRH_AB1EBASIS35Y#0001</v>
       </c>
-      <c r="F164" s="13">
+      <c r="F164" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>2.3523999999999996E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G164" s="13">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
         <v>0</v>
       </c>
       <c r="H164" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I164" s="12">
         <v>40</v>
@@ -9420,11 +9420,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>54525</v>
+        <v>54539</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9445,7 +9445,7 @@
       </c>
       <c r="F165" s="13">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>2.3789999999999999E-2</v>
+        <v>2.3379999999999998E-2</v>
       </c>
       <c r="G165" s="13">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -9462,11 +9462,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>56349</v>
+        <v>56363</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9487,7 +9487,7 @@
       </c>
       <c r="F166" s="13">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>2.4070000000000001E-2</v>
+        <v>2.3629999999999998E-2</v>
       </c>
       <c r="G166" s="13">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -9504,11 +9504,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>60002</v>
+        <v>60016</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9529,7 +9529,7 @@
       </c>
       <c r="F167" s="6">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>2.4289999999999999E-2</v>
+        <v>2.3850000000000003E-2</v>
       </c>
       <c r="G167" s="6">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -9546,11 +9546,11 @@
       </c>
       <c r="K167" s="4">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="L167" s="3">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>63654</v>
+        <v>63668</v>
       </c>
     </row>
   </sheetData>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="E2" s="41">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>2.7929999999999999E-3</v>
+        <v>2.6749999999999999E-3</v>
       </c>
       <c r="F2" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -9631,14 +9631,14 @@
       </c>
       <c r="G2" s="40">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H2" s="39">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41740</v>
+        <v>41754</v>
       </c>
       <c r="I2" s="34">
-        <v>0.99999224172685797</v>
+        <v>0.99998498240509814</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -9653,7 +9653,7 @@
       </c>
       <c r="E3" s="41">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>2.385E-3</v>
+        <v>2.5040000000000001E-3</v>
       </c>
       <c r="F3" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -9661,14 +9661,14 @@
       </c>
       <c r="G3" s="40">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H3" s="39">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41746</v>
+        <v>41761</v>
       </c>
       <c r="I3" s="34">
-        <v>0.99995362715054092</v>
+        <v>0.99993677192256725</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -9683,7 +9683,7 @@
       </c>
       <c r="E4" s="41">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>2.552E-3</v>
+        <v>2.575E-3</v>
       </c>
       <c r="F4" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -9691,14 +9691,14 @@
       </c>
       <c r="G4" s="40">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H4" s="39">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41753</v>
+        <v>41767</v>
       </c>
       <c r="I4" s="34">
-        <v>0.99990076540402273</v>
+        <v>0.99989228474667791</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -9713,7 +9713,7 @@
       </c>
       <c r="E5" s="41">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>2.5820000000000001E-3</v>
+        <v>2.4989999999999999E-3</v>
       </c>
       <c r="F5" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -9721,14 +9721,14 @@
       </c>
       <c r="G5" s="40">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H5" s="39">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41761</v>
+        <v>41774</v>
       </c>
       <c r="I5" s="34">
-        <v>0.99984223600451505</v>
+        <v>0.99984666020220625</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -9744,7 +9744,7 @@
       </c>
       <c r="E6" s="41">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>2.5100000000000001E-3</v>
+        <v>2.4599999999999999E-3</v>
       </c>
       <c r="F6" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -9752,20 +9752,20 @@
       </c>
       <c r="G6" s="40">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H6" s="39">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41771</v>
+        <v>41785</v>
       </c>
       <c r="I6" s="34">
-        <v>0.99977693865635309</v>
+        <v>0.99977379564515612</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_RateHelpersSelected#0001</v>
+        <v>EUR_YC1MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="43" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -9776,7 +9776,7 @@
       </c>
       <c r="E7" s="41">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>2.48E-3</v>
+        <v>2.4199999999999998E-3</v>
       </c>
       <c r="F7" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -9784,14 +9784,14 @@
       </c>
       <c r="G7" s="40">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H7" s="39">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41800</v>
+        <v>41814</v>
       </c>
       <c r="I7" s="34">
-        <v>0.99957994277377538</v>
+        <v>0.99958251779310814</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -9800,7 +9800,7 @@
       </c>
       <c r="E8" s="41">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>2.3999999999999998E-3</v>
+        <v>2.33E-3</v>
       </c>
       <c r="F8" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -9808,14 +9808,14 @@
       </c>
       <c r="G8" s="40">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H8" s="39">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41830</v>
+        <v>41844</v>
       </c>
       <c r="I8" s="34">
-        <v>0.99939366933590257</v>
+        <v>0.99940376093674921</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="E9" s="41">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>2.33E-3</v>
+        <v>2.2599999999999999E-3</v>
       </c>
       <c r="F9" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -9832,14 +9832,14 @@
       </c>
       <c r="G9" s="40">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H9" s="39">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41862</v>
+        <v>41876</v>
       </c>
       <c r="I9" s="34">
-        <v>0.99920448282722285</v>
+        <v>0.99922078221618127</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -9848,7 +9848,7 @@
       </c>
       <c r="E10" s="41">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>2.2799999999999999E-3</v>
+        <v>2.2100000000000002E-3</v>
       </c>
       <c r="F10" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -9856,14 +9856,14 @@
       </c>
       <c r="G10" s="40">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41892</v>
+        <v>41906</v>
       </c>
       <c r="I10" s="34">
-        <v>0.99903182988076833</v>
+        <v>0.99905394850777562</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -9872,7 +9872,7 @@
       </c>
       <c r="E11" s="41">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.2300000000000002E-3</v>
+        <v>2.16E-3</v>
       </c>
       <c r="F11" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -9880,14 +9880,14 @@
       </c>
       <c r="G11" s="40">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41922</v>
+        <v>41936</v>
       </c>
       <c r="I11" s="34">
-        <v>0.99886754536804057</v>
+        <v>0.99889547260814293</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E12" s="41">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.1800000000000001E-3</v>
+        <v>2.1199999999999999E-3</v>
       </c>
       <c r="F12" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -9904,14 +9904,14 @@
       </c>
       <c r="G12" s="40">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41953</v>
+        <v>41967</v>
       </c>
       <c r="I12" s="34">
-        <v>0.99870557028066476</v>
+        <v>0.99873357791086537</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -9920,7 +9920,7 @@
       </c>
       <c r="E13" s="41">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>2.14E-3</v>
+        <v>2.0800000000000003E-3</v>
       </c>
       <c r="F13" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -9928,14 +9928,14 @@
       </c>
       <c r="G13" s="40">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>41983</v>
+        <v>41997</v>
       </c>
       <c r="I13" s="34">
-        <v>0.99855137486384515</v>
+        <v>0.99858436881090107</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -9944,7 +9944,7 @@
       </c>
       <c r="E14" s="41">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>2.1199999999999999E-3</v>
+        <v>2.0500000000000002E-3</v>
       </c>
       <c r="F14" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -9952,14 +9952,14 @@
       </c>
       <c r="G14" s="40">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42016</v>
+        <v>42030</v>
       </c>
       <c r="I14" s="34">
-        <v>0.99837107483091936</v>
+        <v>0.99841722242720166</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -9968,7 +9968,7 @@
       </c>
       <c r="E15" s="41">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>2.0900000000000003E-3</v>
+        <v>2.0300000000000001E-3</v>
       </c>
       <c r="F15" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -9976,14 +9976,14 @@
       </c>
       <c r="G15" s="40">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42045</v>
+        <v>42059</v>
       </c>
       <c r="I15" s="34">
-        <v>0.99822622754936052</v>
+        <v>0.99826951403896391</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -9992,7 +9992,7 @@
       </c>
       <c r="E16" s="41">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>2.0600000000000002E-3</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="F16" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -10000,14 +10000,14 @@
       </c>
       <c r="G16" s="40">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42073</v>
+        <v>42087</v>
       </c>
       <c r="I16" s="34">
-        <v>0.99809195392893324</v>
+        <v>0.99812137877765428</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
@@ -10016,7 +10016,7 @@
       </c>
       <c r="E17" s="41">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>2.0500000000000002E-3</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="F17" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -10024,14 +10024,14 @@
       </c>
       <c r="G17" s="40">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H17" s="39">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42104</v>
+        <v>42118</v>
       </c>
       <c r="I17" s="34">
-        <v>0.99792529693468424</v>
+        <v>0.99794802768439361</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.2">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="E18" s="41">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>2.4399999999999999E-3</v>
+        <v>2.4299999999999999E-3</v>
       </c>
       <c r="F18" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10048,14 +10048,14 @@
       </c>
       <c r="G18" s="40">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H18" s="39">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42471</v>
+        <v>42485</v>
       </c>
       <c r="I18" s="34">
-        <v>0.99512918968712594</v>
+        <v>0.99514154202135197</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.2">
@@ -10064,7 +10064,7 @@
       </c>
       <c r="E19" s="41">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>3.4199999999999999E-3</v>
+        <v>3.4399999999999995E-3</v>
       </c>
       <c r="F19" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10072,14 +10072,14 @@
       </c>
       <c r="G19" s="40">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H19" s="39">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42835</v>
+        <v>42849</v>
       </c>
       <c r="I19" s="34">
-        <v>0.9897980640701457</v>
+        <v>0.98973094871982348</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.2">
@@ -10088,7 +10088,7 @@
       </c>
       <c r="E20" s="41">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>4.9399999999999999E-3</v>
+        <v>5.0400000000000002E-3</v>
       </c>
       <c r="F20" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10096,14 +10096,14 @@
       </c>
       <c r="G20" s="40">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H20" s="39">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43200</v>
+        <v>43214</v>
       </c>
       <c r="I20" s="34">
-        <v>0.98042338923519279</v>
+        <v>0.98002203565065238</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.2">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="E21" s="41">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>6.6699999999999997E-3</v>
+        <v>6.8400000000000006E-3</v>
       </c>
       <c r="F21" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10120,14 +10120,14 @@
       </c>
       <c r="G21" s="40">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H21" s="39">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43565</v>
+        <v>43579</v>
       </c>
       <c r="I21" s="34">
-        <v>0.96712268037641902</v>
+        <v>0.96628622671003273</v>
       </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.2">
@@ -10136,7 +10136,7 @@
       </c>
       <c r="E22" s="41">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>8.5100000000000019E-3</v>
+        <v>8.6599999999999993E-3</v>
       </c>
       <c r="F22" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10144,14 +10144,14 @@
       </c>
       <c r="G22" s="40">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H22" s="39">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43935</v>
+        <v>43945</v>
       </c>
       <c r="I22" s="34">
-        <v>0.94988780333385592</v>
+        <v>0.94910661608755631</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.2">
@@ -10160,7 +10160,7 @@
       </c>
       <c r="E23" s="41">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.03E-2</v>
+        <v>1.042E-2</v>
       </c>
       <c r="F23" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10168,14 +10168,14 @@
       </c>
       <c r="G23" s="40">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H23" s="39">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44298</v>
+        <v>44312</v>
       </c>
       <c r="I23" s="34">
-        <v>0.92983438090221915</v>
+        <v>0.92904155424146895</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.2">
@@ -10184,7 +10184,7 @@
       </c>
       <c r="E24" s="41">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.2019999999999999E-2</v>
+        <v>1.2100000000000001E-2</v>
       </c>
       <c r="F24" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10192,14 +10192,14 @@
       </c>
       <c r="G24" s="40">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H24" s="39">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44662</v>
+        <v>44676</v>
       </c>
       <c r="I24" s="34">
-        <v>0.9072562233071525</v>
+        <v>0.90667593598939278</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.2">
@@ -10208,7 +10208,7 @@
       </c>
       <c r="E25" s="41">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>1.359E-2</v>
+        <v>1.3650000000000001E-2</v>
       </c>
       <c r="F25" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10216,14 +10216,14 @@
       </c>
       <c r="G25" s="40">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H25" s="39">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>45027</v>
+        <v>45040</v>
       </c>
       <c r="I25" s="34">
-        <v>0.88315554699157728</v>
+        <v>0.88272380356824309</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.2">
@@ -10232,7 +10232,7 @@
       </c>
       <c r="E26" s="41">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>1.5010000000000001E-2</v>
+        <v>1.506E-2</v>
       </c>
       <c r="F26" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10240,14 +10240,14 @@
       </c>
       <c r="G26" s="40">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H26" s="39">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>45392</v>
+        <v>45406</v>
       </c>
       <c r="I26" s="34">
-        <v>0.85811843309647773</v>
+        <v>0.85771282228252244</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.2">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="E27" s="41">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>1.7449999999999997E-2</v>
+        <v>1.7419999999999998E-2</v>
       </c>
       <c r="F27" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10264,14 +10264,14 @@
       </c>
       <c r="G27" s="40">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H27" s="39">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>46122</v>
+        <v>46136</v>
       </c>
       <c r="I27" s="34">
-        <v>0.8064891589386477</v>
+        <v>0.80690489015656197</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.2">
@@ -10280,7 +10280,7 @@
       </c>
       <c r="E28" s="41">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.0029999999999999E-2</v>
+        <v>1.993E-2</v>
       </c>
       <c r="F28" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10288,14 +10288,14 @@
       </c>
       <c r="G28" s="40">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H28" s="39">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>47218</v>
+        <v>47232</v>
       </c>
       <c r="I28" s="34">
-        <v>0.73246046860770697</v>
+        <v>0.73383488266547703</v>
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.2">
@@ -10304,7 +10304,7 @@
       </c>
       <c r="E29" s="41">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.214E-2</v>
+        <v>2.1920000000000002E-2</v>
       </c>
       <c r="F29" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10312,14 +10312,14 @@
       </c>
       <c r="G29" s="40">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H29" s="39">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>49045</v>
+        <v>49058</v>
       </c>
       <c r="I29" s="34">
-        <v>0.63021283046955834</v>
+        <v>0.633689647811297</v>
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.2">
@@ -10328,7 +10328,7 @@
       </c>
       <c r="E30" s="41">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.2940000000000002E-2</v>
+        <v>2.265E-2</v>
       </c>
       <c r="F30" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -10336,14 +10336,14 @@
       </c>
       <c r="G30" s="40">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H30" s="39">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>50872</v>
+        <v>50885</v>
       </c>
       <c r="I30" s="34">
-        <v>0.5502179909385031</v>
+        <v>0.55520578802236686</v>
       </c>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.2">
@@ -10352,7 +10352,7 @@
       </c>
       <c r="E31" s="41">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.3259999999999999E-2</v>
+        <v>2.2910000000000003E-2</v>
       </c>
       <c r="F31" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -10360,23 +10360,23 @@
       </c>
       <c r="G31" s="40">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H31" s="39">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>52698</v>
+        <v>52712</v>
       </c>
       <c r="I31" s="34">
-        <v>0.48466114479568162</v>
+        <v>0.49100393839768003</v>
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D32" s="42" t="str">
-        <v>EUR_YC1MRH_AB1EBASIS35Y</v>
+        <v>EUR_YC1MRH_AB1EBASIS40Y</v>
       </c>
       <c r="E32" s="41">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.3523999999999996E-2</v>
+        <v>2.3379999999999998E-2</v>
       </c>
       <c r="F32" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -10384,23 +10384,23 @@
       </c>
       <c r="G32" s="40">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H32" s="39">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>54525</v>
+        <v>56363</v>
       </c>
       <c r="I32" s="34">
-        <v>0.42597243825868708</v>
+        <v>0.38048678011084192</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D33" s="42" t="str">
-        <v>EUR_YC1MRH_AB1EBASIS40Y</v>
+        <v>EUR_YC1MRH_AB1EBASIS50Y</v>
       </c>
       <c r="E33" s="41">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.3789999999999999E-2</v>
+        <v>2.3629999999999998E-2</v>
       </c>
       <c r="F33" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -10408,23 +10408,23 @@
       </c>
       <c r="G33" s="40">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H33" s="39">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>56349</v>
+        <v>60016</v>
       </c>
       <c r="I33" s="34">
-        <v>0.37272866361081824</v>
+        <v>0.29543183212712798</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D34" s="42" t="str">
-        <v>EUR_YC1MRH_AB1EBASIS50Y</v>
+        <v>EUR_YC1MRH_AB1EBASIS60Y</v>
       </c>
       <c r="E34" s="41">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.4070000000000001E-2</v>
+        <v>2.3850000000000003E-2</v>
       </c>
       <c r="F34" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -10432,38 +10432,38 @@
       </c>
       <c r="G34" s="40">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41739</v>
+        <v>41753</v>
       </c>
       <c r="H34" s="39">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>60002</v>
+        <v>63668</v>
       </c>
       <c r="I34" s="34">
-        <v>0.28741559811628115</v>
+        <v>0.22762105274163486</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D35" s="42" t="str">
-        <v>EUR_YC1MRH_AB1EBASIS60Y</v>
-      </c>
-      <c r="E35" s="41">
+      <c r="D35" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E35" s="41" t="e">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.4289999999999999E-2</v>
-      </c>
-      <c r="F35" s="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F35" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="40">
+        <v>--</v>
+      </c>
+      <c r="G35" s="40" t="e">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41739</v>
-      </c>
-      <c r="H35" s="39">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H35" s="39" t="e">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>63654</v>
-      </c>
-      <c r="I35" s="34">
-        <v>0.2203744773058621</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I35" s="34" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>